<commit_message>
large number of updates
</commit_message>
<xml_diff>
--- a/Hedge Funds.xlsx
+++ b/Hedge Funds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE1FE3F-4AE7-4C0D-8419-818EBFFB338C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2706D17A-32C7-487A-88D2-2D3C920A0AA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26430" yWindow="420" windowWidth="24300" windowHeight="20700" xr2:uid="{18689D26-F1F3-46B4-82BE-041D095397EB}"/>
+    <workbookView xWindow="-32205" yWindow="2070" windowWidth="26985" windowHeight="17820" xr2:uid="{18689D26-F1F3-46B4-82BE-041D095397EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hedge" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,7 @@
     8.2B notional</t>
       </text>
     </comment>
-    <comment ref="P64" authorId="19" shapeId="0" xr:uid="{66BA6FAB-F596-46B8-A685-34D82A73F4B0}">
+    <comment ref="P65" authorId="19" shapeId="0" xr:uid="{66BA6FAB-F596-46B8-A685-34D82A73F4B0}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -287,7 +287,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="1326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1931" uniqueCount="1330">
   <si>
     <t>Name</t>
   </si>
@@ -4265,6 +4265,18 @@
   </si>
   <si>
     <t>Cevian</t>
+  </si>
+  <si>
+    <t>Scion</t>
+  </si>
+  <si>
+    <t>Michael Burry</t>
+  </si>
+  <si>
+    <t>Boaz Weinstein</t>
+  </si>
+  <si>
+    <t>Credit</t>
   </si>
 </sst>
 </file>
@@ -4772,7 +4784,7 @@
   <threadedComment ref="P38" dT="2024-03-25T13:19:55.75" personId="{4F866D09-A2D3-41DA-A24C-20DE51662D93}" id="{A95428F5-F28F-4EF2-9805-1BA4B0BC6E31}">
     <text>8.2B notional</text>
   </threadedComment>
-  <threadedComment ref="P64" dT="2024-03-25T00:15:40.04" personId="{4F866D09-A2D3-41DA-A24C-20DE51662D93}" id="{66BA6FAB-F596-46B8-A685-34D82A73F4B0}">
+  <threadedComment ref="P65" dT="2024-03-25T00:15:40.04" personId="{4F866D09-A2D3-41DA-A24C-20DE51662D93}" id="{66BA6FAB-F596-46B8-A685-34D82A73F4B0}">
     <text>11.5B notional</text>
   </threadedComment>
 </ThreadedComments>
@@ -4811,13 +4823,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E8001A6-1B33-4EEE-B2A7-E66E0A0975B5}">
-  <dimension ref="A2:BH227"/>
+  <dimension ref="A2:BH228"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U20" sqref="U20"/>
+      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5135,7 +5147,7 @@
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A5">
-        <f t="shared" ref="A5:A75" si="1">+A4+1</f>
+        <f t="shared" ref="A5:A76" si="1">+A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -6605,1821 +6617,1822 @@
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49">
-        <f t="shared" si="1"/>
-        <v>47</v>
+        <f>+A133+1</f>
+        <v>97</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C49" t="s">
-        <v>1210</v>
-      </c>
-      <c r="P49" s="4">
-        <v>5415.6385790000004</v>
-      </c>
-      <c r="Q49" s="4">
-        <v>5748.0698949999996</v>
+        <v>1328</v>
       </c>
       <c r="R49" s="4">
-        <v>6010.5106290000003</v>
+        <v>6014.5163499999999</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>106</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50">
-        <f t="shared" si="1"/>
-        <v>48</v>
+        <f>+A48+1</f>
+        <v>47</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>27</v>
+        <v>152</v>
       </c>
       <c r="C50" t="s">
-        <v>47</v>
-      </c>
-      <c r="K50" s="4">
-        <v>5379.8770000000004</v>
+        <v>1210</v>
       </c>
       <c r="P50" s="4">
-        <v>5022.5581860000002</v>
+        <v>5415.6385790000004</v>
       </c>
       <c r="Q50" s="4">
-        <v>5972.2947789999998</v>
+        <v>5748.0698949999996</v>
       </c>
       <c r="R50" s="4">
-        <v>6007.4277890000003</v>
+        <v>6010.5106290000003</v>
       </c>
       <c r="S50" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="T50" s="6" t="s">
-        <v>218</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51">
         <f t="shared" si="1"/>
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C51" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="K51" s="4">
-        <v>5387</v>
+        <v>5379.8770000000004</v>
       </c>
       <c r="P51" s="4">
-        <v>5007.2440530000003</v>
+        <v>5022.5581860000002</v>
       </c>
       <c r="Q51" s="4">
-        <v>5459.959793</v>
+        <v>5972.2947789999998</v>
       </c>
       <c r="R51" s="4">
-        <v>5064.5262670000002</v>
+        <v>6007.4277890000003</v>
       </c>
       <c r="S51" s="6" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="T51" s="6" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52">
         <f t="shared" si="1"/>
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C52" t="s">
-        <v>45</v>
-      </c>
-      <c r="J52" s="4">
-        <v>4050.0909999999999</v>
+        <v>58</v>
       </c>
       <c r="K52" s="4">
-        <v>4439.2</v>
+        <v>5387</v>
       </c>
       <c r="P52" s="4">
-        <v>4979.7658250000004</v>
+        <v>5007.2440530000003</v>
       </c>
       <c r="Q52" s="4">
-        <v>5321.4750329999997</v>
+        <v>5459.959793</v>
       </c>
       <c r="R52" s="4">
-        <v>5272.5897709999999</v>
+        <v>5064.5262670000002</v>
       </c>
       <c r="S52" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="T52" s="6" t="s">
-        <v>222</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>1306</v>
+        <v>25</v>
+      </c>
+      <c r="C53" t="s">
+        <v>45</v>
+      </c>
+      <c r="J53" s="4">
+        <v>4050.0909999999999</v>
+      </c>
+      <c r="K53" s="4">
+        <v>4439.2</v>
       </c>
       <c r="P53" s="4">
-        <v>3025.7837439999998</v>
+        <v>4979.7658250000004</v>
       </c>
       <c r="Q53" s="4">
-        <v>3653</v>
+        <v>5321.4750329999997</v>
       </c>
       <c r="R53" s="4">
-        <v>5004.8059999999996</v>
+        <v>5272.5897709999999</v>
+      </c>
+      <c r="S53" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="T53" s="6" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>1312</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1313</v>
+        <v>1306</v>
+      </c>
+      <c r="P54" s="4">
+        <v>3025.7837439999998</v>
+      </c>
+      <c r="Q54" s="4">
+        <v>3653</v>
       </c>
       <c r="R54" s="4">
-        <v>5080.8122750000002</v>
+        <v>5004.8059999999996</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55">
         <f t="shared" si="1"/>
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>39</v>
+        <v>1312</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
-      </c>
-      <c r="K55" s="4">
-        <v>8031.8270000000002</v>
-      </c>
-      <c r="P55" s="4">
-        <v>4723.1373450000001</v>
-      </c>
-      <c r="Q55" s="4">
-        <v>5131.2977549999996</v>
+        <v>1313</v>
       </c>
       <c r="R55" s="4">
-        <v>5303.7028410000003</v>
-      </c>
-      <c r="S55" s="6" t="s">
-        <v>99</v>
+        <v>5080.8122750000002</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>211</v>
+        <v>39</v>
+      </c>
+      <c r="C56" t="s">
+        <v>33</v>
+      </c>
+      <c r="K56" s="4">
+        <v>8031.8270000000002</v>
+      </c>
+      <c r="P56" s="4">
+        <v>4723.1373450000001</v>
+      </c>
+      <c r="Q56" s="4">
+        <v>5131.2977549999996</v>
       </c>
       <c r="R56" s="4">
-        <v>4601.3203059999996</v>
+        <v>5303.7028410000003</v>
+      </c>
+      <c r="S56" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57">
         <f t="shared" si="1"/>
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>705</v>
-      </c>
-      <c r="C57" t="s">
-        <v>706</v>
-      </c>
-      <c r="P57" s="4">
-        <v>4655.038055</v>
-      </c>
-      <c r="Q57" s="4">
-        <v>5053.8065829999996</v>
+        <v>211</v>
       </c>
       <c r="R57" s="4">
-        <v>4019.1749329999998</v>
+        <v>4601.3203059999996</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>109</v>
+        <v>705</v>
       </c>
       <c r="C58" t="s">
-        <v>655</v>
+        <v>706</v>
       </c>
       <c r="P58" s="4">
-        <v>4585.0370000000003</v>
+        <v>4655.038055</v>
       </c>
       <c r="Q58" s="4">
-        <v>3650.7759999999998</v>
+        <v>5053.8065829999996</v>
       </c>
       <c r="R58" s="4">
-        <v>3634.1010000000001</v>
-      </c>
-      <c r="S58" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="T58" s="6" t="s">
-        <v>223</v>
+        <v>4019.1749329999998</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59">
         <f t="shared" si="1"/>
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
+      </c>
+      <c r="C59" t="s">
+        <v>655</v>
       </c>
       <c r="P59" s="4">
-        <v>4370.8550519999999</v>
+        <v>4585.0370000000003</v>
       </c>
       <c r="Q59" s="4">
-        <v>5836.1265380000004</v>
+        <v>3650.7759999999998</v>
       </c>
       <c r="R59" s="4">
-        <v>4883.5933199999999</v>
+        <v>3634.1010000000001</v>
+      </c>
+      <c r="S59" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="T59" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60">
         <f t="shared" si="1"/>
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C60" t="s">
-        <v>53</v>
-      </c>
-      <c r="K60" s="4">
-        <v>3445.66</v>
+        <v>111</v>
       </c>
       <c r="P60" s="4">
-        <v>4481.9567360000001</v>
+        <v>4370.8550519999999</v>
       </c>
       <c r="Q60" s="4">
-        <v>5757.9581449999996</v>
+        <v>5836.1265380000004</v>
       </c>
       <c r="R60" s="4">
-        <v>4199.4415429999999</v>
-      </c>
-      <c r="S60" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="T60" s="6" t="s">
-        <v>223</v>
+        <v>4883.5933199999999</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61">
         <f t="shared" si="1"/>
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>78</v>
+        <v>29</v>
+      </c>
+      <c r="C61" t="s">
+        <v>53</v>
+      </c>
+      <c r="K61" s="4">
+        <v>3445.66</v>
       </c>
       <c r="P61" s="4">
-        <v>3938.719184</v>
+        <v>4481.9567360000001</v>
       </c>
       <c r="Q61" s="4">
-        <v>4466.283023</v>
+        <v>5757.9581449999996</v>
       </c>
       <c r="R61" s="4">
-        <v>4796.3262439999999</v>
+        <v>4199.4415429999999</v>
+      </c>
+      <c r="S61" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="T61" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="C62" t="s">
-        <v>654</v>
+        <v>78</v>
       </c>
       <c r="P62" s="4">
-        <v>2994.3490000000002</v>
+        <v>3938.719184</v>
       </c>
       <c r="Q62" s="4">
-        <v>3491.0940839999998</v>
+        <v>4466.283023</v>
       </c>
       <c r="R62" s="4">
-        <v>3350.3836879999999</v>
-      </c>
-      <c r="S62" s="6" t="s">
-        <v>104</v>
+        <v>4796.3262439999999</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63">
         <f t="shared" si="1"/>
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>189</v>
+        <v>651</v>
+      </c>
+      <c r="C63" t="s">
+        <v>654</v>
       </c>
       <c r="P63" s="4">
-        <v>4995.9489999999996</v>
+        <v>2994.3490000000002</v>
       </c>
       <c r="Q63" s="4">
-        <v>4543.0252979999996</v>
+        <v>3491.0940839999998</v>
       </c>
       <c r="R63" s="4">
-        <v>3556.2966700000002</v>
+        <v>3350.3836879999999</v>
       </c>
       <c r="S63" s="6" t="s">
-        <v>1308</v>
+        <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64">
         <f t="shared" si="1"/>
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>669</v>
-      </c>
-      <c r="C64" t="s">
-        <v>670</v>
+        <v>189</v>
       </c>
       <c r="P64" s="4">
-        <v>3284.2082740000001</v>
+        <v>4995.9489999999996</v>
       </c>
       <c r="Q64" s="4">
-        <v>18987.033237</v>
+        <v>4543.0252979999996</v>
       </c>
       <c r="R64" s="4">
-        <v>15970.332716000001</v>
+        <v>3556.2966700000002</v>
       </c>
       <c r="S64" s="6" t="s">
-        <v>99</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="65" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A65">
         <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="B65" t="s">
-        <v>1305</v>
+        <v>62</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="C65" t="s">
+        <v>670</v>
+      </c>
+      <c r="P65" s="4">
+        <v>3284.2082740000001</v>
+      </c>
+      <c r="Q65" s="4">
+        <v>18987.033237</v>
       </c>
       <c r="R65" s="4">
-        <v>4625</v>
+        <v>15970.332716000001</v>
+      </c>
+      <c r="S65" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A66">
         <f t="shared" si="1"/>
-        <v>64</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="P66" s="4">
-        <v>4062.169985</v>
-      </c>
-      <c r="Q66" s="4">
-        <v>3938.8463550000001</v>
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>1305</v>
       </c>
       <c r="R66" s="4">
-        <v>3322.3777700000001</v>
-      </c>
-      <c r="S66" s="6" t="s">
-        <v>106</v>
+        <v>4625</v>
       </c>
     </row>
     <row r="67" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A67">
         <f t="shared" si="1"/>
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="K67" s="4">
-        <v>1100.212</v>
+        <v>684</v>
       </c>
       <c r="P67" s="4">
-        <v>2334.1559999999999</v>
+        <v>4062.169985</v>
       </c>
       <c r="Q67" s="4">
-        <v>2197.568025</v>
+        <v>3938.8463550000001</v>
       </c>
       <c r="R67" s="4">
-        <v>2050.2866260000001</v>
+        <v>3322.3777700000001</v>
       </c>
       <c r="S67" s="6" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="68" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A68">
         <f t="shared" si="1"/>
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>1139</v>
-      </c>
-      <c r="C68" t="s">
-        <v>1140</v>
+        <v>56</v>
+      </c>
+      <c r="K68" s="4">
+        <v>1100.212</v>
       </c>
       <c r="P68" s="4">
-        <v>3923.913</v>
+        <v>2334.1559999999999</v>
       </c>
       <c r="Q68" s="4">
-        <v>4080.4180000000001</v>
+        <v>2197.568025</v>
       </c>
       <c r="R68" s="4">
-        <v>3613.4749999999999</v>
+        <v>2050.2866260000001</v>
+      </c>
+      <c r="S68" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A69">
         <f t="shared" si="1"/>
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>1316</v>
+        <v>1139</v>
       </c>
       <c r="C69" t="s">
-        <v>1317</v>
+        <v>1140</v>
       </c>
       <c r="P69" s="4">
-        <v>2722.6707569999999</v>
+        <v>3923.913</v>
       </c>
       <c r="Q69" s="4">
-        <v>3102.7736410000002</v>
+        <v>4080.4180000000001</v>
       </c>
       <c r="R69" s="4">
-        <v>3187.7679090000001</v>
-      </c>
-      <c r="S69" s="6" t="s">
-        <v>106</v>
+        <v>3613.4749999999999</v>
       </c>
     </row>
     <row r="70" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A70">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>204</v>
+        <v>1316</v>
+      </c>
+      <c r="C70" t="s">
+        <v>1317</v>
+      </c>
+      <c r="P70" s="4">
+        <v>2722.6707569999999</v>
+      </c>
+      <c r="Q70" s="4">
+        <v>3102.7736410000002</v>
       </c>
       <c r="R70" s="4">
-        <v>2925.13985</v>
+        <v>3187.7679090000001</v>
+      </c>
+      <c r="S70" s="6" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A71">
         <f t="shared" si="1"/>
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>1314</v>
+        <v>204</v>
       </c>
       <c r="R71" s="4">
-        <v>2919.2836120000002</v>
+        <v>2925.13985</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A72">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>1321</v>
-      </c>
-      <c r="C72" t="s">
-        <v>1322</v>
+        <v>1314</v>
       </c>
       <c r="R72" s="4">
-        <v>2722.2935520000001</v>
-      </c>
-      <c r="V72">
-        <v>2011</v>
+        <v>2919.2836120000002</v>
       </c>
     </row>
     <row r="73" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A73">
         <f t="shared" si="1"/>
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>1303</v>
+        <v>1321</v>
       </c>
       <c r="C73" t="s">
-        <v>64</v>
-      </c>
-      <c r="K73" s="4">
-        <v>1412.152</v>
-      </c>
-      <c r="P73" s="4">
-        <v>2047.9987269999999</v>
-      </c>
-      <c r="Q73" s="4"/>
+        <v>1322</v>
+      </c>
       <c r="R73" s="4">
-        <v>2044.4063249999999</v>
-      </c>
-      <c r="S73" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="T73" s="6" t="s">
-        <v>223</v>
+        <v>2722.2935520000001</v>
+      </c>
+      <c r="V73">
+        <v>2011</v>
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A74">
         <f t="shared" si="1"/>
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>60</v>
+        <v>1303</v>
+      </c>
+      <c r="C74" t="s">
+        <v>64</v>
+      </c>
+      <c r="K74" s="4">
+        <v>1412.152</v>
       </c>
       <c r="P74" s="4">
-        <v>1765.235518</v>
-      </c>
-      <c r="Q74" s="4">
-        <v>1182.369925</v>
-      </c>
+        <v>2047.9987269999999</v>
+      </c>
+      <c r="Q74" s="4"/>
       <c r="R74" s="4">
-        <v>1063.3875740000001</v>
+        <v>2044.4063249999999</v>
       </c>
       <c r="S74" s="6" t="s">
-        <v>99</v>
+        <v>102</v>
+      </c>
+      <c r="T74" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A75">
         <f t="shared" si="1"/>
-        <v>73</v>
-      </c>
-      <c r="B75" t="s">
-        <v>1302</v>
+        <v>72</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P75" s="4">
+        <v>1765.235518</v>
+      </c>
+      <c r="Q75" s="4">
+        <v>1182.369925</v>
       </c>
       <c r="R75" s="4">
-        <v>2709.2641100000001</v>
+        <v>1063.3875740000001</v>
+      </c>
+      <c r="S75" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A76">
-        <f t="shared" ref="A76:A107" si="2">+A75+1</f>
-        <v>74</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="P76" s="4">
-        <v>1549.0588190000001</v>
-      </c>
-      <c r="Q76" s="4">
-        <v>1829.5737349999999</v>
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="B76" t="s">
+        <v>1302</v>
       </c>
       <c r="R76" s="4">
-        <v>1709.7065090000001</v>
+        <v>2709.2641100000001</v>
       </c>
     </row>
     <row r="77" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A77">
-        <f t="shared" si="2"/>
-        <v>75</v>
+        <f t="shared" ref="A77:A109" si="2">+A76+1</f>
+        <v>74</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="P77" s="4">
-        <v>1339.16731</v>
+        <v>1549.0588190000001</v>
       </c>
       <c r="Q77" s="4">
-        <v>1523.792498</v>
+        <v>1829.5737349999999</v>
       </c>
       <c r="R77" s="4">
-        <v>1259.015003</v>
+        <v>1709.7065090000001</v>
       </c>
     </row>
     <row r="78" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A78">
         <f t="shared" si="2"/>
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="K78" s="4">
-        <v>1264.742</v>
+        <v>97</v>
       </c>
       <c r="P78" s="4">
-        <v>1106.539</v>
+        <v>1339.16731</v>
       </c>
       <c r="Q78" s="4">
-        <v>886.72607700000003</v>
+        <v>1523.792498</v>
       </c>
       <c r="R78" s="4">
-        <v>862.98003200000005</v>
-      </c>
-      <c r="S78" s="6" t="s">
-        <v>104</v>
+        <v>1259.015003</v>
       </c>
     </row>
     <row r="79" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A79">
         <f t="shared" si="2"/>
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>672</v>
+        <v>50</v>
+      </c>
+      <c r="K79" s="4">
+        <v>1264.742</v>
       </c>
       <c r="P79" s="4">
-        <v>1101.3968339999999</v>
+        <v>1106.539</v>
       </c>
       <c r="Q79" s="4">
-        <v>1333.7237869999999</v>
+        <v>886.72607700000003</v>
       </c>
       <c r="R79" s="4">
-        <v>1412.847262</v>
-      </c>
-      <c r="U79" s="8" t="s">
-        <v>673</v>
+        <v>862.98003200000005</v>
+      </c>
+      <c r="S79" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A80">
         <f t="shared" si="2"/>
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C80" t="s">
-        <v>73</v>
-      </c>
-      <c r="K80" s="4">
-        <v>815.42100000000005</v>
+        <v>672</v>
       </c>
       <c r="P80" s="4">
-        <v>1082.240147</v>
+        <v>1101.3968339999999</v>
       </c>
       <c r="Q80" s="4">
-        <v>960.44607399999995</v>
+        <v>1333.7237869999999</v>
       </c>
       <c r="R80" s="4">
-        <v>981.87468000000001</v>
-      </c>
-      <c r="S80" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="T80" s="6" t="s">
-        <v>223</v>
+        <v>1412.847262</v>
+      </c>
+      <c r="U80" s="8" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A81">
         <f t="shared" si="2"/>
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>208</v>
+        <v>51</v>
       </c>
       <c r="C81" t="s">
-        <v>1211</v>
+        <v>73</v>
+      </c>
+      <c r="K81" s="4">
+        <v>815.42100000000005</v>
       </c>
       <c r="P81" s="4">
-        <v>2093.868226</v>
+        <v>1082.240147</v>
       </c>
       <c r="Q81" s="4">
-        <v>2279.648201</v>
+        <v>960.44607399999995</v>
       </c>
       <c r="R81" s="4">
-        <v>1731.086869</v>
+        <v>981.87468000000001</v>
+      </c>
+      <c r="S81" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="T81" s="6" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A82">
         <f t="shared" si="2"/>
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>657</v>
+        <v>208</v>
       </c>
       <c r="C82" t="s">
-        <v>658</v>
+        <v>1211</v>
       </c>
       <c r="P82" s="4">
-        <v>1018.739</v>
+        <v>2093.868226</v>
       </c>
       <c r="Q82" s="4">
-        <v>1345.1919969999999</v>
+        <v>2279.648201</v>
       </c>
       <c r="R82" s="4">
-        <v>1304.5958989999999</v>
-      </c>
-      <c r="S82" s="6" t="s">
-        <v>104</v>
+        <v>1731.086869</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A83">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>1311</v>
+        <v>657</v>
+      </c>
+      <c r="C83" t="s">
+        <v>658</v>
       </c>
       <c r="P83" s="4">
-        <v>1150.712</v>
+        <v>1018.739</v>
       </c>
       <c r="Q83" s="4">
-        <v>1225.489343</v>
+        <v>1345.1919969999999</v>
       </c>
       <c r="R83" s="4">
-        <v>1211.5763959999999</v>
+        <v>1304.5958989999999</v>
+      </c>
+      <c r="S83" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A84">
         <f t="shared" si="2"/>
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>1271</v>
+        <v>1311</v>
+      </c>
+      <c r="P84" s="4">
+        <v>1150.712</v>
+      </c>
+      <c r="Q84" s="4">
+        <v>1225.489343</v>
       </c>
       <c r="R84" s="4">
-        <v>840.39369999999997</v>
+        <v>1211.5763959999999</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A85">
         <f t="shared" si="2"/>
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C85" t="s">
-        <v>1315</v>
+        <v>1271</v>
       </c>
       <c r="R85" s="4">
-        <v>778.69210999999996</v>
+        <v>840.39369999999997</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A86">
         <f t="shared" si="2"/>
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="K86" s="4">
-        <v>1092.9059999999999</v>
-      </c>
-      <c r="P86" s="4">
-        <v>808.65300000000002</v>
-      </c>
-      <c r="Q86" s="4">
-        <v>913.78966700000001</v>
+        <v>199</v>
+      </c>
+      <c r="C86" t="s">
+        <v>1315</v>
       </c>
       <c r="R86" s="4">
-        <v>675.32564400000001</v>
-      </c>
-      <c r="S86" s="6" t="s">
-        <v>102</v>
+        <v>778.69210999999996</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A87">
         <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-      <c r="B87" t="s">
-        <v>1304</v>
+        <v>84</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K87" s="4">
+        <v>1092.9059999999999</v>
+      </c>
+      <c r="P87" s="4">
+        <v>808.65300000000002</v>
+      </c>
+      <c r="Q87" s="4">
+        <v>913.78966700000001</v>
       </c>
       <c r="R87" s="4">
-        <v>529.70181100000002</v>
+        <v>675.32564400000001</v>
+      </c>
+      <c r="S87" s="6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A88">
         <f t="shared" si="2"/>
-        <v>86</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>1307</v>
-      </c>
-      <c r="P88" s="4">
-        <v>273.69799999999998</v>
-      </c>
-      <c r="Q88" s="4">
-        <v>272.0761</v>
+        <v>85</v>
+      </c>
+      <c r="B88" t="s">
+        <v>1304</v>
       </c>
       <c r="R88" s="4">
-        <v>353.461074</v>
+        <v>529.70181100000002</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A89">
         <f t="shared" si="2"/>
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>142</v>
+        <v>1307</v>
       </c>
       <c r="P89" s="4">
-        <v>741.80454199999997</v>
-      </c>
-      <c r="Q89" s="4"/>
-      <c r="R89" s="4"/>
+        <v>273.69799999999998</v>
+      </c>
+      <c r="Q89" s="4">
+        <v>272.0761</v>
+      </c>
+      <c r="R89" s="4">
+        <v>353.461074</v>
+      </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A90">
         <f t="shared" si="2"/>
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="P90" s="4">
-        <v>332.71594900000002</v>
-      </c>
-      <c r="Q90" s="4"/>
-      <c r="R90" s="4"/>
-      <c r="S90" s="6" t="s">
-        <v>665</v>
+        <v>1326</v>
+      </c>
+      <c r="C90" t="s">
+        <v>1327</v>
+      </c>
+      <c r="R90" s="4">
+        <v>52</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A91">
         <f t="shared" si="2"/>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C91" t="s">
-        <v>72</v>
-      </c>
-      <c r="K91" s="4">
-        <v>799.58</v>
+        <v>142</v>
       </c>
       <c r="P91" s="4">
-        <v>109.111527</v>
+        <v>741.80454199999997</v>
       </c>
       <c r="Q91" s="4"/>
       <c r="R91" s="4"/>
-      <c r="S91" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="T91" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="U91" s="8" t="s">
-        <v>656</v>
-      </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A92">
         <f t="shared" si="2"/>
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="P92" s="4">
-        <v>70.898508000000007</v>
+        <v>332.71594900000002</v>
       </c>
       <c r="Q92" s="4"/>
       <c r="R92" s="4"/>
+      <c r="S92" s="6" t="s">
+        <v>665</v>
+      </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A93">
         <f t="shared" si="2"/>
-        <v>91</v>
-      </c>
-      <c r="B93" t="s">
-        <v>61</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C93" t="s">
+        <v>72</v>
+      </c>
+      <c r="K93" s="4">
+        <v>799.58</v>
+      </c>
+      <c r="P93" s="4">
+        <v>109.111527</v>
+      </c>
+      <c r="Q93" s="4"/>
+      <c r="R93" s="4"/>
       <c r="S93" s="6" t="s">
-        <v>659</v>
+        <v>106</v>
+      </c>
+      <c r="T93" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="U93" s="8" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A94">
         <f t="shared" si="2"/>
-        <v>92</v>
-      </c>
-      <c r="B94" t="s">
-        <v>108</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="P94" s="4">
+        <v>70.898508000000007</v>
+      </c>
+      <c r="Q94" s="4"/>
+      <c r="R94" s="4"/>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A95">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>113</v>
+        <v>61</v>
+      </c>
+      <c r="S95" s="6" t="s">
+        <v>659</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A96">
         <f t="shared" si="2"/>
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <f t="shared" si="2"/>
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>69</v>
-      </c>
-      <c r="C97" t="s">
-        <v>700</v>
+        <v>113</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <f t="shared" si="2"/>
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <f t="shared" si="2"/>
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>116</v>
+        <v>69</v>
+      </c>
+      <c r="C99" t="s">
+        <v>700</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <f t="shared" si="2"/>
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>682</v>
+        <v>74</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <f t="shared" si="2"/>
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102">
         <f t="shared" si="2"/>
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>119</v>
+        <v>682</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103">
         <f t="shared" si="2"/>
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104">
         <f t="shared" si="2"/>
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105">
         <f t="shared" si="2"/>
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106">
         <f t="shared" si="2"/>
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107">
         <f t="shared" si="2"/>
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108">
-        <f t="shared" ref="A108:A159" si="3">+A107+1</f>
-        <v>106</v>
+        <f t="shared" si="2"/>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109">
-        <f t="shared" si="3"/>
-        <v>107</v>
+        <f t="shared" si="2"/>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110">
-        <f t="shared" si="3"/>
-        <v>108</v>
+        <f t="shared" ref="A110:A160" si="3">+A109+1</f>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111">
         <f t="shared" si="3"/>
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112">
         <f t="shared" si="3"/>
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>1325</v>
+        <v>131</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113">
         <f t="shared" si="3"/>
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114">
         <f t="shared" si="3"/>
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>134</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115">
         <f t="shared" si="3"/>
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116">
         <f t="shared" si="3"/>
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117">
         <f t="shared" si="3"/>
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118">
         <f t="shared" si="3"/>
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119">
         <f t="shared" si="3"/>
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120">
         <f t="shared" si="3"/>
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121">
         <f t="shared" si="3"/>
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122">
         <f t="shared" si="3"/>
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123">
         <f t="shared" si="3"/>
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124">
         <f t="shared" si="3"/>
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>1298</v>
+        <v>143</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125">
-        <f t="shared" si="3"/>
-        <v>123</v>
+        <f>+A90+1</f>
+        <v>88</v>
       </c>
       <c r="B125" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126">
         <f t="shared" si="3"/>
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="B126" t="s">
-        <v>146</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127">
         <f t="shared" si="3"/>
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="B127" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128">
         <f t="shared" si="3"/>
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="B128" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129">
         <f t="shared" si="3"/>
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="B129" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="B130" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131">
         <f t="shared" si="3"/>
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="B131" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132">
         <f t="shared" si="3"/>
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="B132" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133">
         <f t="shared" si="3"/>
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="B133" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134">
-        <f t="shared" si="3"/>
-        <v>132</v>
+        <f>+A49+1</f>
+        <v>98</v>
       </c>
       <c r="B134" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135">
         <f t="shared" si="3"/>
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="B135" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136">
         <f t="shared" si="3"/>
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="B136" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137">
         <f t="shared" si="3"/>
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B137" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138">
         <f t="shared" si="3"/>
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="B138" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="B139" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140">
         <f t="shared" si="3"/>
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="B140" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141">
         <f t="shared" si="3"/>
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="B141" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="B142" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143">
         <f t="shared" si="3"/>
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="B143" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144">
         <f t="shared" si="3"/>
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="B144" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145">
         <f t="shared" si="3"/>
-        <v>143</v>
+        <v>109</v>
       </c>
       <c r="B145" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146">
         <f t="shared" si="3"/>
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="B146" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147">
         <f t="shared" si="3"/>
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="B147" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>112</v>
       </c>
       <c r="B148" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149">
         <f t="shared" si="3"/>
-        <v>147</v>
+        <v>113</v>
       </c>
       <c r="B149" t="s">
-        <v>1119</v>
-      </c>
-      <c r="C149" t="s">
-        <v>1120</v>
+        <v>170</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150">
         <f t="shared" si="3"/>
-        <v>148</v>
+        <v>114</v>
       </c>
       <c r="B150" t="s">
-        <v>171</v>
+        <v>1119</v>
+      </c>
+      <c r="C150" t="s">
+        <v>1120</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151">
         <f t="shared" si="3"/>
-        <v>149</v>
+        <v>115</v>
       </c>
       <c r="B151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152">
         <f t="shared" si="3"/>
-        <v>150</v>
+        <v>116</v>
       </c>
       <c r="B152" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153">
         <f t="shared" si="3"/>
-        <v>151</v>
+        <v>117</v>
       </c>
       <c r="B153" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="B154" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155">
         <f t="shared" si="3"/>
-        <v>153</v>
+        <v>119</v>
       </c>
       <c r="B155" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156">
         <f t="shared" si="3"/>
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="B156" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>121</v>
       </c>
       <c r="B157" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158">
         <f t="shared" si="3"/>
-        <v>156</v>
+        <v>122</v>
       </c>
       <c r="B158" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159">
         <f t="shared" si="3"/>
-        <v>157</v>
+        <v>123</v>
       </c>
       <c r="B159" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160">
-        <f t="shared" ref="A160:A189" si="4">+A159+1</f>
-        <v>158</v>
+        <f t="shared" si="3"/>
+        <v>124</v>
       </c>
       <c r="B160" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161">
-        <f t="shared" si="4"/>
-        <v>159</v>
+        <f t="shared" ref="A161:A190" si="4">+A160+1</f>
+        <v>125</v>
       </c>
       <c r="B161" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162">
         <f t="shared" si="4"/>
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="B162" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163">
         <f t="shared" si="4"/>
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="B163" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164">
         <f t="shared" si="4"/>
-        <v>162</v>
+        <v>128</v>
       </c>
       <c r="B164" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165">
         <f t="shared" si="4"/>
-        <v>163</v>
+        <v>129</v>
       </c>
       <c r="B165" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166">
         <f t="shared" si="4"/>
-        <v>164</v>
+        <v>130</v>
       </c>
       <c r="B166" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167">
         <f t="shared" si="4"/>
-        <v>165</v>
+        <v>131</v>
       </c>
       <c r="B167" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168">
         <f t="shared" si="4"/>
-        <v>166</v>
+        <v>132</v>
       </c>
       <c r="B168" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169">
         <f t="shared" si="4"/>
-        <v>167</v>
+        <v>133</v>
       </c>
       <c r="B169" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170">
         <f t="shared" si="4"/>
-        <v>168</v>
+        <v>134</v>
       </c>
       <c r="B170" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171">
         <f t="shared" si="4"/>
-        <v>169</v>
+        <v>135</v>
       </c>
       <c r="B171" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172">
         <f t="shared" si="4"/>
-        <v>170</v>
+        <v>136</v>
       </c>
       <c r="B172" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173">
         <f t="shared" si="4"/>
-        <v>171</v>
+        <v>137</v>
       </c>
       <c r="B173" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174">
         <f t="shared" si="4"/>
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="B174" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175">
         <f t="shared" si="4"/>
-        <v>173</v>
+        <v>139</v>
       </c>
       <c r="B175" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176">
         <f t="shared" si="4"/>
-        <v>174</v>
+        <v>140</v>
       </c>
       <c r="B176" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A177">
         <f t="shared" si="4"/>
-        <v>175</v>
+        <v>141</v>
       </c>
       <c r="B177" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A178">
         <f t="shared" si="4"/>
-        <v>176</v>
+        <v>142</v>
       </c>
       <c r="B178" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A179">
         <f t="shared" si="4"/>
-        <v>177</v>
+        <v>143</v>
       </c>
       <c r="B179" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A180">
         <f t="shared" si="4"/>
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="B180" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A181">
         <f t="shared" si="4"/>
-        <v>179</v>
+        <v>145</v>
       </c>
       <c r="B181" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A182">
         <f t="shared" si="4"/>
-        <v>180</v>
+        <v>146</v>
       </c>
       <c r="B182" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A183">
         <f t="shared" si="4"/>
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="B183" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A184">
         <f t="shared" si="4"/>
-        <v>182</v>
+        <v>148</v>
       </c>
       <c r="B184" t="s">
-        <v>233</v>
-      </c>
-      <c r="C184" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A185">
         <f t="shared" si="4"/>
-        <v>183</v>
+        <v>149</v>
       </c>
       <c r="B185" t="s">
-        <v>704</v>
+        <v>233</v>
+      </c>
+      <c r="C185" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A186">
         <f t="shared" si="4"/>
-        <v>184</v>
+        <v>150</v>
       </c>
       <c r="B186" t="s">
-        <v>1126</v>
+        <v>704</v>
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A187">
         <f t="shared" si="4"/>
-        <v>185</v>
+        <v>151</v>
       </c>
       <c r="B187" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A188">
         <f t="shared" si="4"/>
-        <v>186</v>
+        <v>152</v>
       </c>
       <c r="B188" t="s">
-        <v>1324</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A189">
         <f t="shared" si="4"/>
-        <v>187</v>
+        <v>153</v>
       </c>
       <c r="B189" t="s">
+        <v>1324</v>
+      </c>
+    </row>
+    <row r="190" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+      <c r="B190" t="s">
         <v>1212</v>
       </c>
-    </row>
-    <row r="191" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B191" s="22" t="s">
-        <v>1214</v>
-      </c>
-      <c r="D191" s="23"/>
-      <c r="E191" s="24"/>
-      <c r="F191" s="24"/>
-      <c r="G191" s="24"/>
-      <c r="H191" s="24"/>
-      <c r="I191" s="23"/>
-      <c r="J191" s="23"/>
-      <c r="K191" s="23"/>
-      <c r="L191" s="23"/>
-      <c r="M191" s="23"/>
-      <c r="N191" s="23"/>
-      <c r="O191" s="23"/>
-      <c r="P191" s="23"/>
-      <c r="Q191" s="23"/>
-      <c r="R191" s="23"/>
-      <c r="S191" s="25"/>
-      <c r="T191" s="25"/>
-      <c r="U191" s="26"/>
     </row>
     <row r="192" spans="1:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B192" s="22" t="s">
-        <v>62</v>
+        <v>1214</v>
       </c>
       <c r="D192" s="23"/>
       <c r="E192" s="24"/>
@@ -8436,187 +8449,210 @@
       <c r="P192" s="23"/>
       <c r="Q192" s="23"/>
       <c r="R192" s="23"/>
-      <c r="S192" s="25" t="s">
-        <v>656</v>
-      </c>
+      <c r="S192" s="25"/>
       <c r="T192" s="25"/>
       <c r="U192" s="26"/>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:21" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B193" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D193" s="23"/>
+      <c r="E193" s="24"/>
+      <c r="F193" s="24"/>
+      <c r="G193" s="24"/>
+      <c r="H193" s="24"/>
+      <c r="I193" s="23"/>
+      <c r="J193" s="23"/>
+      <c r="K193" s="23"/>
+      <c r="L193" s="23"/>
+      <c r="M193" s="23"/>
+      <c r="N193" s="23"/>
+      <c r="O193" s="23"/>
+      <c r="P193" s="23"/>
+      <c r="Q193" s="23"/>
+      <c r="R193" s="23"/>
+      <c r="S193" s="25" t="s">
+        <v>656</v>
+      </c>
+      <c r="T193" s="25"/>
+      <c r="U193" s="26"/>
+    </row>
+    <row r="194" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B194" s="22" t="s">
         <v>1272</v>
       </c>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B194" s="22" t="s">
+    <row r="195" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B195" s="22" t="s">
         <v>1273</v>
       </c>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B195" s="22" t="s">
+    <row r="196" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B196" s="22" t="s">
         <v>1274</v>
       </c>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B196" s="22" t="s">
+    <row r="197" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B197" s="22" t="s">
         <v>1275</v>
       </c>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B197" s="22" t="s">
+    <row r="198" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B198" s="22" t="s">
         <v>1276</v>
       </c>
-      <c r="C197" t="s">
+      <c r="C198" t="s">
         <v>1323</v>
       </c>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B198" s="22" t="s">
+    <row r="199" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B199" s="22" t="s">
         <v>1277</v>
       </c>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B199" s="22" t="s">
+    <row r="200" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B200" s="22" t="s">
         <v>1278</v>
       </c>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B200" s="22" t="s">
+    <row r="201" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B201" s="22" t="s">
         <v>1279</v>
       </c>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B201" s="22" t="s">
+    <row r="202" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B202" s="22" t="s">
         <v>1280</v>
       </c>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B202" s="22" t="s">
+    <row r="203" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B203" s="22" t="s">
         <v>1281</v>
       </c>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B203" s="22" t="s">
+    <row r="204" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B204" s="22" t="s">
         <v>727</v>
       </c>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B204" s="22" t="s">
+    <row r="205" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B205" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B205" s="22" t="s">
+    <row r="206" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B206" s="22" t="s">
         <v>1282</v>
       </c>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B206" s="22" t="s">
+    <row r="207" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B207" s="22" t="s">
         <v>1283</v>
       </c>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B207" s="22" t="s">
+    <row r="208" spans="2:21" x14ac:dyDescent="0.2">
+      <c r="B208" s="22" t="s">
         <v>196</v>
-      </c>
-    </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B208" s="22" t="s">
-        <v>1284</v>
       </c>
     </row>
     <row r="209" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B209" s="22" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="210" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B210" s="22" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="211" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B211" s="22" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="212" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B212" s="22" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="213" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B213" s="22" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="214" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B214" s="22" t="s">
-        <v>43</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="215" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B215" s="22" t="s">
-        <v>1290</v>
+        <v>43</v>
       </c>
     </row>
     <row r="216" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B216" s="22" t="s">
-        <v>1291</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="217" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B217" s="22" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="218" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B218" s="22" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="219" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B219" s="22" t="s">
-        <v>188</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="220" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B220" s="22" t="s">
-        <v>1294</v>
+        <v>188</v>
       </c>
     </row>
     <row r="221" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B221" s="22" t="s">
-        <v>190</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="222" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B222" s="22" t="s">
-        <v>1295</v>
+        <v>190</v>
       </c>
     </row>
     <row r="223" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B223" s="22" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="224" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B224" s="22" t="s">
-        <v>108</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="225" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B225" s="22" t="s">
-        <v>194</v>
+        <v>108</v>
       </c>
     </row>
     <row r="226" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B226" s="22" t="s">
-        <v>1309</v>
+        <v>194</v>
       </c>
     </row>
     <row r="227" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B227" s="22" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B228" s="22" t="s">
         <v>1310</v>
       </c>
     </row>
@@ -8644,8 +8680,8 @@
     <hyperlink ref="I4" r:id="rId20" display="https://www.sec.gov/Archives/edgar/data/1273087/000127308722000070/0001273087-22-000070-index.htm" xr:uid="{C6E348DF-7E26-4EA5-BD9B-6BC16802E3AE}"/>
     <hyperlink ref="B14" r:id="rId21" xr:uid="{2AF557B7-F280-4AD5-919A-E7B6E05A794A}"/>
     <hyperlink ref="K14" r:id="rId22" display="https://www.sec.gov/Archives/edgar/data/1218710/000095012322012462/0000950123-22-012462-index.htm" xr:uid="{96D48D17-D545-4DC3-AE94-F0461E6C9B1C}"/>
-    <hyperlink ref="B55" r:id="rId23" display="Och-Ziff" xr:uid="{508856E8-03F7-419A-8B01-3BF187BC71E0}"/>
-    <hyperlink ref="K55" r:id="rId24" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012322012327/0000950123-22-012327-index.htm" xr:uid="{F608A635-5184-4DEE-8F2D-2ACBAD2F5CD4}"/>
+    <hyperlink ref="B56" r:id="rId23" display="Och-Ziff" xr:uid="{508856E8-03F7-419A-8B01-3BF187BC71E0}"/>
+    <hyperlink ref="K56" r:id="rId24" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012322012327/0000950123-22-012327-index.htm" xr:uid="{F608A635-5184-4DEE-8F2D-2ACBAD2F5CD4}"/>
     <hyperlink ref="B16" r:id="rId25" xr:uid="{66D4608B-A6D7-418A-8388-7E1FBF305BE1}"/>
     <hyperlink ref="K16" r:id="rId26" display="https://www.sec.gov/Archives/edgar/data/1103804/000110380422000006/0001103804-22-000006-index.htm" xr:uid="{D0A1B2F0-25D5-499E-9B2D-9D789D8813C2}"/>
     <hyperlink ref="J16" r:id="rId27" display="https://www.sec.gov/Archives/edgar/data/1103804/000110380422000004/0001103804-22-000004-index.htm" xr:uid="{B34C0065-3749-409F-80F9-B99DD5A24C32}"/>
@@ -8655,27 +8691,27 @@
     <hyperlink ref="K17" r:id="rId31" display="https://www.sec.gov/Archives/edgar/data/1135730/000091957422006523/0000919574-22-006523-index.htm" xr:uid="{1ED343BB-50A1-407A-82B8-A90D870C430D}"/>
     <hyperlink ref="B21" r:id="rId32" xr:uid="{720247CE-D1BC-42AE-94E0-B6B5D2E25FBD}"/>
     <hyperlink ref="K21" r:id="rId33" display="https://www.sec.gov/Archives/edgar/data/1061165/000090266422004869/0000902664-22-004869-index.htm" xr:uid="{DC68DFAB-C6BA-4465-8767-433D8A9E46BF}"/>
-    <hyperlink ref="B52" r:id="rId34" xr:uid="{963BA984-F42D-4353-9337-DFF49A956B89}"/>
-    <hyperlink ref="K52" r:id="rId35" display="https://www.sec.gov/Archives/edgar/data/934639/000094787122001169/0000947871-22-001169-index.htm" xr:uid="{265165E6-B392-4436-A2B2-09315DA20D93}"/>
-    <hyperlink ref="J52" r:id="rId36" display="https://www.sec.gov/Archives/edgar/data/934639/000094787122000896/0000947871-22-000896-index.htm" xr:uid="{162CA86C-8012-4F25-BAC3-47938851EEDA}"/>
+    <hyperlink ref="B53" r:id="rId34" xr:uid="{963BA984-F42D-4353-9337-DFF49A956B89}"/>
+    <hyperlink ref="K53" r:id="rId35" display="https://www.sec.gov/Archives/edgar/data/934639/000094787122001169/0000947871-22-001169-index.htm" xr:uid="{265165E6-B392-4436-A2B2-09315DA20D93}"/>
+    <hyperlink ref="J53" r:id="rId36" display="https://www.sec.gov/Archives/edgar/data/934639/000094787122000896/0000947871-22-000896-index.htm" xr:uid="{162CA86C-8012-4F25-BAC3-47938851EEDA}"/>
     <hyperlink ref="B13" r:id="rId37" xr:uid="{8B12E547-810C-44D6-8E3B-5938CC54481E}"/>
     <hyperlink ref="K13" r:id="rId38" display="https://www.sec.gov/Archives/edgar/data/1478735/000091957422006648/0000919574-22-006648-index.htm" xr:uid="{FCAEF47B-B6A4-411C-BA41-7368B80D112C}"/>
-    <hyperlink ref="B50" r:id="rId39" xr:uid="{325FD0A5-B199-4FBD-B3E9-54B63AB4885F}"/>
-    <hyperlink ref="K50" r:id="rId40" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957422006703/0000919574-22-006703-index.htm" xr:uid="{3058CEA3-FF25-4F78-9648-8BFB7D327351}"/>
+    <hyperlink ref="B51" r:id="rId39" xr:uid="{325FD0A5-B199-4FBD-B3E9-54B63AB4885F}"/>
+    <hyperlink ref="K51" r:id="rId40" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957422006703/0000919574-22-006703-index.htm" xr:uid="{3058CEA3-FF25-4F78-9648-8BFB7D327351}"/>
     <hyperlink ref="B27" r:id="rId41" xr:uid="{2EF5ED89-B2CB-46ED-8A9F-DFADD3D9628C}"/>
     <hyperlink ref="K27" r:id="rId42" display="https://www.sec.gov/Archives/edgar/data/1263508/000110465922118527/0001104659-22-118527-index.htm" xr:uid="{2337DE61-D888-457B-B014-96A2B42AF57D}"/>
-    <hyperlink ref="B60" r:id="rId43" xr:uid="{B6B2A5A3-6AED-4C29-B804-4C0E43A93695}"/>
-    <hyperlink ref="K60" r:id="rId44" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297522000502/0001012975-22-000502-index.htm" xr:uid="{9BA31348-D395-48AA-8E7B-99A357433FFF}"/>
+    <hyperlink ref="B61" r:id="rId43" xr:uid="{B6B2A5A3-6AED-4C29-B804-4C0E43A93695}"/>
+    <hyperlink ref="K61" r:id="rId44" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297522000502/0001012975-22-000502-index.htm" xr:uid="{9BA31348-D395-48AA-8E7B-99A357433FFF}"/>
     <hyperlink ref="B42" r:id="rId45" xr:uid="{2998E001-3A83-4857-B1DA-5642E83F2662}"/>
     <hyperlink ref="K42" r:id="rId46" display="https://www.sec.gov/Archives/edgar/data/1493215/000149315222032245/0001493152-22-032245-index.htm" xr:uid="{5479AC29-F188-4F2F-8B18-E98009817328}"/>
     <hyperlink ref="B33" r:id="rId47" xr:uid="{2433CCA6-D76A-4D6C-BA8C-E071F51C5FBC}"/>
     <hyperlink ref="K33" r:id="rId48" display="https://www.sec.gov/Archives/edgar/data/1601086/000131586322000788/0001315863-22-000788-index.htm" xr:uid="{6FD1223B-3BC6-460A-856D-449D11BA229F}"/>
-    <hyperlink ref="B51" r:id="rId49" xr:uid="{47E85512-9C4B-4C85-890F-F392A3B5B19B}"/>
-    <hyperlink ref="K51" r:id="rId50" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266122002553/0001172661-22-002553-index.htm" xr:uid="{76ECED4E-5561-49E4-B352-C0A1791CBC9F}"/>
+    <hyperlink ref="B52" r:id="rId49" xr:uid="{47E85512-9C4B-4C85-890F-F392A3B5B19B}"/>
+    <hyperlink ref="K52" r:id="rId50" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266122002553/0001172661-22-002553-index.htm" xr:uid="{76ECED4E-5561-49E4-B352-C0A1791CBC9F}"/>
     <hyperlink ref="B23" r:id="rId51" xr:uid="{456AFC9C-67D1-4C5B-A738-F41E8BB0A3F8}"/>
     <hyperlink ref="K23" r:id="rId52" display="https://www.sec.gov/Archives/edgar/data/1336528/000117266122002568/0001172661-22-002568-index.htm" xr:uid="{AB660963-74B3-447E-B466-575FDB35D8E9}"/>
-    <hyperlink ref="B73" r:id="rId53" display="Greenlight" xr:uid="{71F66E8E-9791-41B4-AC86-48058DF35E75}"/>
-    <hyperlink ref="K73" r:id="rId54" display="https://www.sec.gov/Archives/edgar/data/1079114/000117266122002565/0001172661-22-002565-index.htm" xr:uid="{E94B7EED-875B-46A4-8E57-7D5B779E81EF}"/>
+    <hyperlink ref="B74" r:id="rId53" display="Greenlight" xr:uid="{71F66E8E-9791-41B4-AC86-48058DF35E75}"/>
+    <hyperlink ref="K74" r:id="rId54" display="https://www.sec.gov/Archives/edgar/data/1079114/000117266122002565/0001172661-22-002565-index.htm" xr:uid="{E94B7EED-875B-46A4-8E57-7D5B779E81EF}"/>
     <hyperlink ref="B39" r:id="rId55" xr:uid="{AD3731C3-BC02-4663-A447-A96646F1598D}"/>
     <hyperlink ref="K39" r:id="rId56" display="https://www.sec.gov/Archives/edgar/data/1040273/000108514622004128/0001085146-22-004128-index.htm" xr:uid="{6C662106-1AC1-415A-AAA8-790368F414D8}"/>
     <hyperlink ref="B26" r:id="rId57" xr:uid="{2A67F66A-4093-449D-9885-A26114FA4297}"/>
@@ -8684,18 +8720,18 @@
     <hyperlink ref="K7" r:id="rId60" display="https://www.sec.gov/Archives/edgar/data/1009207/000110465922118505/0001104659-22-118505-index.htm" xr:uid="{B226747D-DAB9-4641-B8A3-DE587815AB8E}"/>
     <hyperlink ref="B3" r:id="rId61" xr:uid="{03C7C8D4-ADD7-4E0D-B7EC-36F70D50940E}"/>
     <hyperlink ref="K3" r:id="rId62" display="https://www.sec.gov/Archives/edgar/data/1067983/000095012322012275/0000950123-22-012275-index.htm" xr:uid="{63E4759D-454A-45CD-8B82-CA7005817809}"/>
-    <hyperlink ref="B91" r:id="rId63" xr:uid="{16F94819-F95B-490D-84A3-010976C1D290}"/>
-    <hyperlink ref="K91" r:id="rId64" display="https://www.sec.gov/Archives/edgar/data/1343781/000134378122000007/0001343781-22-000007-index.htm" xr:uid="{220E0C47-6F7C-4608-A00F-F7E03FD8EF04}"/>
-    <hyperlink ref="B86" r:id="rId65" xr:uid="{0C9CCBF7-C4C5-4BA1-A48F-BBF28E20255A}"/>
-    <hyperlink ref="K86" r:id="rId66" display="https://www.sec.gov/Archives/edgar/data/1279150/000121390022072102/0001213900-22-072102-index.htm" xr:uid="{3E480569-E528-4449-AA70-DC9876454290}"/>
-    <hyperlink ref="B78" r:id="rId67" xr:uid="{FAC1DB71-DF8E-47D5-A2AE-69FCC44F0A6A}"/>
-    <hyperlink ref="K78" r:id="rId68" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692322000016/0001306923-22-000016-index.htm" xr:uid="{2F8D6909-71C2-4009-8DAA-3EE7C509F8D2}"/>
-    <hyperlink ref="B80" r:id="rId69" xr:uid="{8C3FDA36-48A7-412B-9D12-4A5DF2BBFB0B}"/>
-    <hyperlink ref="K80" r:id="rId70" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465922013682/0001214659-22-013682-index.htm" xr:uid="{1269CAFA-37F5-45B0-A201-4882036446DA}"/>
+    <hyperlink ref="B93" r:id="rId63" xr:uid="{16F94819-F95B-490D-84A3-010976C1D290}"/>
+    <hyperlink ref="K93" r:id="rId64" display="https://www.sec.gov/Archives/edgar/data/1343781/000134378122000007/0001343781-22-000007-index.htm" xr:uid="{220E0C47-6F7C-4608-A00F-F7E03FD8EF04}"/>
+    <hyperlink ref="B87" r:id="rId65" xr:uid="{0C9CCBF7-C4C5-4BA1-A48F-BBF28E20255A}"/>
+    <hyperlink ref="K87" r:id="rId66" display="https://www.sec.gov/Archives/edgar/data/1279150/000121390022072102/0001213900-22-072102-index.htm" xr:uid="{3E480569-E528-4449-AA70-DC9876454290}"/>
+    <hyperlink ref="B79" r:id="rId67" xr:uid="{FAC1DB71-DF8E-47D5-A2AE-69FCC44F0A6A}"/>
+    <hyperlink ref="K79" r:id="rId68" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692322000016/0001306923-22-000016-index.htm" xr:uid="{2F8D6909-71C2-4009-8DAA-3EE7C509F8D2}"/>
+    <hyperlink ref="B81" r:id="rId69" xr:uid="{8C3FDA36-48A7-412B-9D12-4A5DF2BBFB0B}"/>
+    <hyperlink ref="K81" r:id="rId70" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465922013682/0001214659-22-013682-index.htm" xr:uid="{1269CAFA-37F5-45B0-A201-4882036446DA}"/>
     <hyperlink ref="B40" r:id="rId71" xr:uid="{2717DFCC-DE67-4786-86FE-0640B6C9833F}"/>
     <hyperlink ref="K40" r:id="rId72" display="https://www.sec.gov/Archives/edgar/data/1346824/000110465922118654/xslForm13F_X01/primary_doc.xml" xr:uid="{D6AC2921-0E6F-4591-809D-B87C8EFEF4A3}"/>
-    <hyperlink ref="B67" r:id="rId73" xr:uid="{B09A4DEB-2524-4C20-AC09-D2E3A3FC4C1B}"/>
-    <hyperlink ref="K67" r:id="rId74" display="https://www.sec.gov/edgar/browse/?CIK=1443689" xr:uid="{09CBA0FE-5D1C-458A-92B5-33620ED13533}"/>
+    <hyperlink ref="B68" r:id="rId73" xr:uid="{B09A4DEB-2524-4C20-AC09-D2E3A3FC4C1B}"/>
+    <hyperlink ref="K68" r:id="rId74" display="https://www.sec.gov/edgar/browse/?CIK=1443689" xr:uid="{09CBA0FE-5D1C-458A-92B5-33620ED13533}"/>
     <hyperlink ref="B6" r:id="rId75" xr:uid="{F474C7AE-00F0-498A-B275-6401609757C7}"/>
     <hyperlink ref="K6" r:id="rId76" display="https://www.sec.gov/edgar/browse/?CIK=1595888" xr:uid="{D24115A5-46E1-4B4B-877F-89BAD5D49739}"/>
     <hyperlink ref="J21" r:id="rId77" display="https://www.sec.gov/Archives/edgar/data/1061165/000090266422003974/0000902664-22-003974-index.htm" xr:uid="{75CFDC66-8255-4C14-9AD0-D113538E8F52}"/>
@@ -8717,13 +8753,13 @@
     <hyperlink ref="L21" r:id="rId93" display="https://www.sec.gov/Archives/edgar/data/1061165/000090266423001763/0000902664-23-001763-index.htm" xr:uid="{B48518A6-2D4C-46DE-B029-2B9CEB71105D}"/>
     <hyperlink ref="N5" r:id="rId94" display="https://www.sec.gov/Archives/edgar/data/1423053/000095012323005271/xslForm13F_X02/22950.xml" xr:uid="{CE7F7333-DE83-4738-B300-4059A32946D2}"/>
     <hyperlink ref="M5" r:id="rId95" display="https://www.sec.gov/Archives/edgar/data/1423053/000095012323002617/xslForm13F_X02/20792.xml" xr:uid="{A58332A7-223A-4B25-8867-74A094B6F685}"/>
-    <hyperlink ref="B62" r:id="rId96" xr:uid="{31930E36-435E-BE4D-BEEE-A0AEF9C118DC}"/>
-    <hyperlink ref="B58" r:id="rId97" xr:uid="{AB404BDB-A318-6D49-B45D-720414E210FE}"/>
-    <hyperlink ref="P58" r:id="rId98" display="https://www.sec.gov/Archives/edgar/data/1061768/000156761924000192/xslForm13F_X02/primary_doc.xml" xr:uid="{B94E4385-8FA8-7646-8E61-B396BAF96F3E}"/>
-    <hyperlink ref="B82" r:id="rId99" xr:uid="{40FEA578-F449-324C-8F20-45CB8AB6FCBC}"/>
-    <hyperlink ref="P82" r:id="rId100" display="https://www.sec.gov/Archives/edgar/data/1534261/000091957424001474/xslForm13F_X02/primary_doc.xml" xr:uid="{6EB6BD3F-7A6E-844B-98BD-51EB6E58A1B7}"/>
+    <hyperlink ref="B63" r:id="rId96" xr:uid="{31930E36-435E-BE4D-BEEE-A0AEF9C118DC}"/>
+    <hyperlink ref="B59" r:id="rId97" xr:uid="{AB404BDB-A318-6D49-B45D-720414E210FE}"/>
+    <hyperlink ref="P59" r:id="rId98" display="https://www.sec.gov/Archives/edgar/data/1061768/000156761924000192/xslForm13F_X02/primary_doc.xml" xr:uid="{B94E4385-8FA8-7646-8E61-B396BAF96F3E}"/>
+    <hyperlink ref="B83" r:id="rId99" xr:uid="{40FEA578-F449-324C-8F20-45CB8AB6FCBC}"/>
+    <hyperlink ref="P83" r:id="rId100" display="https://www.sec.gov/Archives/edgar/data/1534261/000091957424001474/xslForm13F_X02/primary_doc.xml" xr:uid="{6EB6BD3F-7A6E-844B-98BD-51EB6E58A1B7}"/>
     <hyperlink ref="P42" r:id="rId101" display="https://www.sec.gov/Archives/edgar/data/1493215/000149315224006286/xslForm13F_X02/primary_doc.xml" xr:uid="{F6580225-B4CA-A748-8BB2-A0E407BEA57F}"/>
-    <hyperlink ref="P60" r:id="rId102" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297524000093/xslForm13F_X02/primary_doc.xml" xr:uid="{8FE0CC6D-B3B1-B243-A602-E633F6C5E621}"/>
+    <hyperlink ref="P61" r:id="rId102" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297524000093/xslForm13F_X02/primary_doc.xml" xr:uid="{8FE0CC6D-B3B1-B243-A602-E633F6C5E621}"/>
     <hyperlink ref="P5" r:id="rId103" display="https://www.sec.gov/Archives/edgar/data/1423053/000095012324002516/xslForm13F_X02/primary_doc.xml" xr:uid="{2286DE1E-2B8D-B247-84AA-10723ECAA2C9}"/>
     <hyperlink ref="P3" r:id="rId104" display="https://www.sec.gov/Archives/edgar/data/1067983/000095012324002518/xslForm13F_X02/primary_doc.xml" xr:uid="{4E0F305B-17C6-3F46-BB23-CDD1F6B60D0B}"/>
     <hyperlink ref="P6" r:id="rId105" display="https://www.sec.gov/Archives/edgar/data/1595888/000159588824000037/xslForm13F_X02/primary_doc.xmlhttps://www.sec.gov/Archives/edgar/data/1595888/000159588824000037/xslForm13F_X02/primary_doc.xml" xr:uid="{204151C5-BC49-2C40-91E4-4F62A3688341}"/>
@@ -8740,30 +8776,30 @@
     <hyperlink ref="P20" r:id="rId116" display="https://www.sec.gov/Archives/edgar/data/1167483/000091957424001349/xslForm13F_X02/primary_doc.xml" xr:uid="{84B0DD05-4802-3F4B-98D1-228F52FFC174}"/>
     <hyperlink ref="P26" r:id="rId117" display="https://www.sec.gov/Archives/edgar/data/1791786/000101359424000185/xslForm13F_X02/primary_doc.xml" xr:uid="{10BCF264-7CDF-7941-A1C6-45F79F56A943}"/>
     <hyperlink ref="P17" r:id="rId118" display="https://www.sec.gov/Archives/edgar/data/1135730/000091957424001118/xslForm13F_X02/primary_doc.xml" xr:uid="{96859F10-C74E-2F47-923F-91BBE9E2B576}"/>
-    <hyperlink ref="P55" r:id="rId119" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012324002531/xslForm13F_X02/primary_doc.xml" xr:uid="{7D39E30F-3607-364C-8CC4-7AF53F8F0AA3}"/>
+    <hyperlink ref="P56" r:id="rId119" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012324002531/xslForm13F_X02/primary_doc.xml" xr:uid="{7D39E30F-3607-364C-8CC4-7AF53F8F0AA3}"/>
     <hyperlink ref="P23" r:id="rId120" display="https://www.sec.gov/Archives/edgar/data/1336528/000117266124001556/xslForm13F_X02/primary_doc.xml" xr:uid="{632606A6-A8B3-F848-A6F2-76932A731A75}"/>
     <hyperlink ref="P33" r:id="rId121" display="https://www.sec.gov/Archives/edgar/data/1601086/000131586324000239/xslForm13F_X02/primary_doc.xml" xr:uid="{E1D6D513-66F6-A94C-87B5-9FE4B1F1F062}"/>
     <hyperlink ref="P39" r:id="rId122" display="https://www.sec.gov/Archives/edgar/data/1040273/000108514624001503/xslForm13F_X02/primary_doc.xml" xr:uid="{0736B7F0-D80A-CC42-A44C-DD2B5A79FD18}"/>
-    <hyperlink ref="P51" r:id="rId123" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266124001461/xslForm13F_X02/primary_doc.xml" xr:uid="{0A82E668-62ED-AD49-BB9B-D5F14C0DD7D7}"/>
-    <hyperlink ref="P50" r:id="rId124" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957424001384/xslForm13F_X02/primary_doc.xml" xr:uid="{6EDB1E41-4367-EB41-BE3C-B79E2F2D9832}"/>
+    <hyperlink ref="P52" r:id="rId123" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266124001461/xslForm13F_X02/primary_doc.xml" xr:uid="{0A82E668-62ED-AD49-BB9B-D5F14C0DD7D7}"/>
+    <hyperlink ref="P51" r:id="rId124" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957424001384/xslForm13F_X02/primary_doc.xml" xr:uid="{6EDB1E41-4367-EB41-BE3C-B79E2F2D9832}"/>
     <hyperlink ref="P40" r:id="rId125" display="https://www.sec.gov/Archives/edgar/data/1346824/000110465924023984/xslForm13F_X02/primary_doc.xml" xr:uid="{C26696FF-0248-C04E-BEC0-1578D46AF98E}"/>
-    <hyperlink ref="P52" r:id="rId126" display="https://www.sec.gov/Archives/edgar/data/934639/000094787124000140/xslForm13F_X02/primary_doc.xml" xr:uid="{9AFCD2C4-5245-A64F-9457-96213DCF1797}"/>
-    <hyperlink ref="P73" r:id="rId127" display="https://www.sec.gov/Archives/edgar/data/1079114/000117266124001512/xslForm13F_X02/primary_doc.xml" xr:uid="{B46332DB-93E6-3149-A4F1-B4EB136FFFD3}"/>
-    <hyperlink ref="P78" r:id="rId128" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692324000002/xslForm13F_X02/primary_doc.xml" xr:uid="{2437CF0F-9F88-B548-B9AA-5E5CD03D1FF3}"/>
-    <hyperlink ref="P67" r:id="rId129" display="https://www.sec.gov/Archives/edgar/data/1443689/000144368924000003/xslForm13F_X02/primary_doc.xml" xr:uid="{233876C2-E934-B94C-A9BE-4574722731EB}"/>
-    <hyperlink ref="P86" r:id="rId130" display="https://www.sec.gov/Archives/edgar/data/1279150/000199937124002312/xslForm13F_X02/primary_doc.xml" xr:uid="{54888D79-11E2-A14D-B41A-C9553C130600}"/>
-    <hyperlink ref="P80" r:id="rId131" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465924002878/xslForm13F_X02/primary_doc.xml" xr:uid="{420C55EB-D070-6348-8FF8-0C2D8C1302C9}"/>
-    <hyperlink ref="P91" r:id="rId132" display="https://www.sec.gov/Archives/edgar/data/1343781/000134378123000001/xslForm13F_X02/primary_doc.xml" xr:uid="{E01B82C3-B0FD-A74F-A10C-2FBF5D0EDF90}"/>
-    <hyperlink ref="B90" r:id="rId133" xr:uid="{6A463FEC-5974-4445-8540-FBD9874A6F2E}"/>
-    <hyperlink ref="P90" r:id="rId134" display="https://www.sec.gov/Archives/edgar/data/1480532/000090514824000714/xslForm13F_X02/primary_doc.xml" xr:uid="{D0D1CB3C-F65B-644A-BEA3-E1CAADC451EE}"/>
-    <hyperlink ref="P74" r:id="rId135" display="https://www.sec.gov/Archives/edgar/data/1290162/000095012324002421/xslForm13F_X02/primary_doc.xml" xr:uid="{EF5C6778-C73D-5641-A311-D195CCD00EC3}"/>
-    <hyperlink ref="B74" r:id="rId136" xr:uid="{5B93D3F1-6081-5742-8962-76B6F05EE3A2}"/>
+    <hyperlink ref="P53" r:id="rId126" display="https://www.sec.gov/Archives/edgar/data/934639/000094787124000140/xslForm13F_X02/primary_doc.xml" xr:uid="{9AFCD2C4-5245-A64F-9457-96213DCF1797}"/>
+    <hyperlink ref="P74" r:id="rId127" display="https://www.sec.gov/Archives/edgar/data/1079114/000117266124001512/xslForm13F_X02/primary_doc.xml" xr:uid="{B46332DB-93E6-3149-A4F1-B4EB136FFFD3}"/>
+    <hyperlink ref="P79" r:id="rId128" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692324000002/xslForm13F_X02/primary_doc.xml" xr:uid="{2437CF0F-9F88-B548-B9AA-5E5CD03D1FF3}"/>
+    <hyperlink ref="P68" r:id="rId129" display="https://www.sec.gov/Archives/edgar/data/1443689/000144368924000003/xslForm13F_X02/primary_doc.xml" xr:uid="{233876C2-E934-B94C-A9BE-4574722731EB}"/>
+    <hyperlink ref="P87" r:id="rId130" display="https://www.sec.gov/Archives/edgar/data/1279150/000199937124002312/xslForm13F_X02/primary_doc.xml" xr:uid="{54888D79-11E2-A14D-B41A-C9553C130600}"/>
+    <hyperlink ref="P81" r:id="rId131" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465924002878/xslForm13F_X02/primary_doc.xml" xr:uid="{420C55EB-D070-6348-8FF8-0C2D8C1302C9}"/>
+    <hyperlink ref="P93" r:id="rId132" display="https://www.sec.gov/Archives/edgar/data/1343781/000134378123000001/xslForm13F_X02/primary_doc.xml" xr:uid="{E01B82C3-B0FD-A74F-A10C-2FBF5D0EDF90}"/>
+    <hyperlink ref="B92" r:id="rId133" xr:uid="{6A463FEC-5974-4445-8540-FBD9874A6F2E}"/>
+    <hyperlink ref="P92" r:id="rId134" display="https://www.sec.gov/Archives/edgar/data/1480532/000090514824000714/xslForm13F_X02/primary_doc.xml" xr:uid="{D0D1CB3C-F65B-644A-BEA3-E1CAADC451EE}"/>
+    <hyperlink ref="P75" r:id="rId135" display="https://www.sec.gov/Archives/edgar/data/1290162/000095012324002421/xslForm13F_X02/primary_doc.xml" xr:uid="{EF5C6778-C73D-5641-A311-D195CCD00EC3}"/>
+    <hyperlink ref="B75" r:id="rId136" xr:uid="{5B93D3F1-6081-5742-8962-76B6F05EE3A2}"/>
     <hyperlink ref="P9" r:id="rId137" display="https://www.sec.gov/Archives/edgar/data/1446194/000144619424000002/xslForm13F_X02/primary_doc.xml" xr:uid="{7C613B92-4B80-AA45-9039-AFF56C0ECC0C}"/>
     <hyperlink ref="B9" r:id="rId138" xr:uid="{EA70B08A-4781-4748-B4CC-EB1EE51971BE}"/>
-    <hyperlink ref="B64" r:id="rId139" xr:uid="{66D7FFAA-AC47-984C-A825-565C92EC7291}"/>
-    <hyperlink ref="P64" r:id="rId140" display="https://www.sec.gov/Archives/edgar/data/1666335/000166633524000002/xslForm13F_X02/primary_doc.xml" xr:uid="{366E98AE-8EE6-534B-8B29-14217BD40599}"/>
-    <hyperlink ref="B79" r:id="rId141" xr:uid="{6889EF5A-BFE8-DB45-8C05-BEB672DBFFD2}"/>
-    <hyperlink ref="P79" r:id="rId142" display="https://www.sec.gov/Archives/edgar/data/1817652/000181765224000002/xslForm13F_X02/primary_doc.xml" xr:uid="{0D004145-9903-9141-AFF5-43D48900DF6C}"/>
+    <hyperlink ref="B65" r:id="rId139" xr:uid="{66D7FFAA-AC47-984C-A825-565C92EC7291}"/>
+    <hyperlink ref="P65" r:id="rId140" display="https://www.sec.gov/Archives/edgar/data/1666335/000166633524000002/xslForm13F_X02/primary_doc.xml" xr:uid="{366E98AE-8EE6-534B-8B29-14217BD40599}"/>
+    <hyperlink ref="B80" r:id="rId141" xr:uid="{6889EF5A-BFE8-DB45-8C05-BEB672DBFFD2}"/>
+    <hyperlink ref="P80" r:id="rId142" display="https://www.sec.gov/Archives/edgar/data/1817652/000181765224000002/xslForm13F_X02/primary_doc.xml" xr:uid="{0D004145-9903-9141-AFF5-43D48900DF6C}"/>
     <hyperlink ref="B11" r:id="rId143" xr:uid="{1679472C-51C1-4C43-AEEC-D7B9CA6AC4BC}"/>
     <hyperlink ref="P11" r:id="rId144" display="https://www.sec.gov/Archives/edgar/data/1318757/000131875724000002/xslForm13F_X02/primary_doc.xml" xr:uid="{A231EBF1-C5BA-8B4E-B62E-7CA9253421FA}"/>
     <hyperlink ref="O17" r:id="rId145" display="https://www.sec.gov/Archives/edgar/data/1135730/000091957423006173/xslForm13F_X02/primary_doc.xml" xr:uid="{B6E0E3A1-CB11-4BB9-B92E-B32EC5F72F78}"/>
@@ -8791,44 +8827,44 @@
     <hyperlink ref="P10" r:id="rId167" display="https://www.sec.gov/Archives/edgar/data/1167557/000108514624001456/xslForm13F_X02/primary_doc.xml" xr:uid="{44DFDFD1-26FB-49F5-BCF9-5B8682308FE9}"/>
     <hyperlink ref="B48" r:id="rId168" xr:uid="{8CE4B88A-0C39-4579-B4F5-6FBF3CC1D963}"/>
     <hyperlink ref="P48" r:id="rId169" display="https://www.sec.gov/Archives/edgar/data/1387322/000138732224000002/xslForm13F_X02/primary_doc.xml" xr:uid="{4CC640F6-0DF4-42AE-B770-8F37D755B90F}"/>
-    <hyperlink ref="B61" r:id="rId170" xr:uid="{1DA1FC49-E258-4701-9E34-019B2E17358F}"/>
-    <hyperlink ref="P61" r:id="rId171" display="https://www.sec.gov/Archives/edgar/data/1352851/000110465924017420/xslForm13F_X02/primary_doc.xml" xr:uid="{6B9556A9-29F7-4E75-86C1-65B0E5139C5B}"/>
+    <hyperlink ref="B62" r:id="rId170" xr:uid="{1DA1FC49-E258-4701-9E34-019B2E17358F}"/>
+    <hyperlink ref="P62" r:id="rId171" display="https://www.sec.gov/Archives/edgar/data/1352851/000110465924017420/xslForm13F_X02/primary_doc.xml" xr:uid="{6B9556A9-29F7-4E75-86C1-65B0E5139C5B}"/>
     <hyperlink ref="B35" r:id="rId172" xr:uid="{B89384A7-75A1-41DB-962F-C2A7A9462D04}"/>
     <hyperlink ref="P35" r:id="rId173" display="https://www.sec.gov/Archives/edgar/data/923093/000095012324002455/xslForm13F_X02/primary_doc.xml" xr:uid="{E3D1EE23-69D1-47FC-A3AB-2EC5865C3801}"/>
     <hyperlink ref="B43" r:id="rId174" xr:uid="{50E1290F-3BC3-4C30-89CE-B39C2D6D14B6}"/>
     <hyperlink ref="P43" r:id="rId175" display="https://www.sec.gov/Archives/edgar/data/1448574/000144857424000001/xslForm13F_X02/primary_doc.xml" xr:uid="{C8EB1DDE-5DFB-49E1-BADE-EE1DB50BFDFE}"/>
-    <hyperlink ref="B92" r:id="rId176" xr:uid="{472BFD61-7C32-4EE6-9B39-4357850D25C6}"/>
-    <hyperlink ref="P92" r:id="rId177" display="https://www.sec.gov/Archives/edgar/data/1218199/000095014224000421/xslForm13F_X02/primary_doc.xml" xr:uid="{5A7B0BAF-24E7-4CD6-925E-241A2F5CC100}"/>
+    <hyperlink ref="B94" r:id="rId176" xr:uid="{472BFD61-7C32-4EE6-9B39-4357850D25C6}"/>
+    <hyperlink ref="P94" r:id="rId177" display="https://www.sec.gov/Archives/edgar/data/1218199/000095014224000421/xslForm13F_X02/primary_doc.xml" xr:uid="{5A7B0BAF-24E7-4CD6-925E-241A2F5CC100}"/>
     <hyperlink ref="B24" r:id="rId178" xr:uid="{9695A6DE-88CA-475B-8766-AAAC0C060A54}"/>
     <hyperlink ref="P24" r:id="rId179" display="https://www.sec.gov/Archives/edgar/data/1410830/000117266124000852/xslForm13F_X02/primary_doc.xml" xr:uid="{4CD33CD4-6BCF-459B-B22D-5D99014AE4F2}"/>
     <hyperlink ref="B28" r:id="rId180" xr:uid="{2DEB3C92-3122-4F61-AD1A-3AA49E2AFC7F}"/>
     <hyperlink ref="P28" r:id="rId181" display="https://www.sec.gov/Archives/edgar/data/1736225/000173622524000003/xslForm13F_X02/primary_doc.xml" xr:uid="{76B6C172-B2FF-4068-A2AA-4421B1ECC5B0}"/>
     <hyperlink ref="B34" r:id="rId182" xr:uid="{3B883934-0164-4E7C-9BA2-4E1E79ECB10D}"/>
     <hyperlink ref="P34" r:id="rId183" display="https://www.sec.gov/Archives/edgar/data/1633313/000110465924023272/xslForm13F_X02/primary_doc.xmlhttps:/www.sec.gov/Archives/edgar/data/1633313/000110465924023272/xslForm13F_X02/primary_doc.xml" xr:uid="{BA056B43-BD39-4C3D-AFB5-A9790C9753A1}"/>
-    <hyperlink ref="B59" r:id="rId184" xr:uid="{A95D8659-3AAC-4BF9-BA55-CB45612B59C6}"/>
-    <hyperlink ref="P59" r:id="rId185" display="https://www.sec.gov/Archives/edgar/data/1595082/000159508224000013/xslForm13F_X02/primary_doc.xml" xr:uid="{0500F989-CCC8-4CED-9BA5-F1ED3D86C922}"/>
+    <hyperlink ref="B60" r:id="rId184" xr:uid="{A95D8659-3AAC-4BF9-BA55-CB45612B59C6}"/>
+    <hyperlink ref="P60" r:id="rId185" display="https://www.sec.gov/Archives/edgar/data/1595082/000159508224000013/xslForm13F_X02/primary_doc.xml" xr:uid="{0500F989-CCC8-4CED-9BA5-F1ED3D86C922}"/>
     <hyperlink ref="B19" r:id="rId186" xr:uid="{EEF25FB9-290F-4C09-B338-B9E51FB69359}"/>
     <hyperlink ref="P19" r:id="rId187" display="https://www.sec.gov/Archives/edgar/data/909661/000090883424000070/xslForm13F_X02/primary_doc.xml" xr:uid="{82CC29D5-64C1-4EF8-85D5-CF77DA408C46}"/>
     <hyperlink ref="B46" r:id="rId188" xr:uid="{56DEF564-A004-40C1-BA0A-D8B6CD4BE1E3}"/>
     <hyperlink ref="P46" r:id="rId189" display="https://www.sec.gov/Archives/edgar/data/1656456/000165645624000001/xslForm13F_X02/primary_doc.xml" xr:uid="{391CBBE9-4862-434A-AC9A-B84D858141D6}"/>
-    <hyperlink ref="B49" r:id="rId190" xr:uid="{77A4FC1B-9BD5-45DE-9F27-F026755CC65F}"/>
-    <hyperlink ref="P49" r:id="rId191" display="https://www.sec.gov/Archives/edgar/data/1009258/000095015924000096/xslForm13F_X02/primary_doc.xml" xr:uid="{4C352723-7D5F-45DD-A8A8-74DC5757A3BF}"/>
+    <hyperlink ref="B50" r:id="rId190" xr:uid="{77A4FC1B-9BD5-45DE-9F27-F026755CC65F}"/>
+    <hyperlink ref="P50" r:id="rId191" display="https://www.sec.gov/Archives/edgar/data/1009258/000095015924000096/xslForm13F_X02/primary_doc.xml" xr:uid="{4C352723-7D5F-45DD-A8A8-74DC5757A3BF}"/>
     <hyperlink ref="B29" r:id="rId192" xr:uid="{079031EF-886C-4963-97A9-00245C3FC571}"/>
     <hyperlink ref="P29" r:id="rId193" display="https://www.sec.gov/Archives/edgar/data/1029160/000090266424001751/xslForm13F_X02/primary_doc.xml" xr:uid="{4F134D78-73D9-46E8-94B8-5A72BAF10562}"/>
-    <hyperlink ref="B76" r:id="rId194" xr:uid="{94B36541-BE14-48E5-AA3B-6538F60B3D3E}"/>
-    <hyperlink ref="P76" r:id="rId195" display="https://www.sec.gov/Archives/edgar/data/1998597/000090266424001588/xslForm13F_X02/primary_doc.xml" xr:uid="{044AAF4F-C172-4481-AE71-F0BE62419751}"/>
+    <hyperlink ref="B77" r:id="rId194" xr:uid="{94B36541-BE14-48E5-AA3B-6538F60B3D3E}"/>
+    <hyperlink ref="P77" r:id="rId195" display="https://www.sec.gov/Archives/edgar/data/1998597/000090266424001588/xslForm13F_X02/primary_doc.xml" xr:uid="{044AAF4F-C172-4481-AE71-F0BE62419751}"/>
     <hyperlink ref="B47" r:id="rId196" xr:uid="{17F81053-FB1E-441E-999B-955EC668BF4C}"/>
     <hyperlink ref="P47" r:id="rId197" display="https://www.sec.gov/Archives/edgar/data/1747057/000117266124000870/xslForm13F_X02/primary_doc.xml" xr:uid="{2D83034F-EFC6-4482-9017-D1C0C61E67A5}"/>
-    <hyperlink ref="B57" r:id="rId198" xr:uid="{156C49F5-13CC-45BF-BBA6-0EB42BBF191A}"/>
-    <hyperlink ref="P57" r:id="rId199" display="https://www.sec.gov/Archives/edgar/data/1319998/000101297524000090/xslForm13F_X02/primary_doc.xml" xr:uid="{B7C97AD8-D74C-4569-A9C4-F89C750EB73D}"/>
+    <hyperlink ref="B58" r:id="rId198" xr:uid="{156C49F5-13CC-45BF-BBA6-0EB42BBF191A}"/>
+    <hyperlink ref="P58" r:id="rId199" display="https://www.sec.gov/Archives/edgar/data/1319998/000101297524000090/xslForm13F_X02/primary_doc.xml" xr:uid="{B7C97AD8-D74C-4569-A9C4-F89C750EB73D}"/>
     <hyperlink ref="B37" r:id="rId200" xr:uid="{DEC6A424-983C-43A2-91B8-2BAE0449565A}"/>
     <hyperlink ref="P37" r:id="rId201" display="https://www.sec.gov/Archives/edgar/data/1107310/000108514624001243/xslForm13F_X02/primary_doc.xml" xr:uid="{61BEEBAE-1B33-46ED-B851-88DC4B65DB0D}"/>
     <hyperlink ref="B25" r:id="rId202" xr:uid="{4110C0AA-9A9F-4DA2-BBCD-4EBDEE61A842}"/>
     <hyperlink ref="P25" r:id="rId203" display="https://www.sec.gov/Archives/edgar/data/1784547/000117266124001100/xslForm13F_X02/primary_doc.xml" xr:uid="{7B68F55D-84EA-498D-A153-7894888EA096}"/>
-    <hyperlink ref="B89" r:id="rId204" xr:uid="{E7004015-E1E1-4319-A273-FC4BD66CC5B2}"/>
-    <hyperlink ref="P89" r:id="rId205" display="https://www.sec.gov/Archives/edgar/data/1390113/000108514624001258/xslForm13F_X02/primary_doc.xml" xr:uid="{8F22AEF2-620D-4165-BE85-2009149A07A4}"/>
-    <hyperlink ref="B77" r:id="rId206" xr:uid="{255B7A8A-E015-4C99-AC90-B3138B786D90}"/>
-    <hyperlink ref="P77" r:id="rId207" display="https://www.sec.gov/Archives/edgar/data/1608485/000091957424001085/xslForm13F_X02/primary_doc.xml" xr:uid="{C1F7B284-A149-4D9A-9E7F-C78AD1418FA9}"/>
+    <hyperlink ref="B91" r:id="rId204" xr:uid="{E7004015-E1E1-4319-A273-FC4BD66CC5B2}"/>
+    <hyperlink ref="P91" r:id="rId205" display="https://www.sec.gov/Archives/edgar/data/1390113/000108514624001258/xslForm13F_X02/primary_doc.xml" xr:uid="{8F22AEF2-620D-4165-BE85-2009149A07A4}"/>
+    <hyperlink ref="B78" r:id="rId206" xr:uid="{255B7A8A-E015-4C99-AC90-B3138B786D90}"/>
+    <hyperlink ref="P78" r:id="rId207" display="https://www.sec.gov/Archives/edgar/data/1608485/000091957424001085/xslForm13F_X02/primary_doc.xml" xr:uid="{C1F7B284-A149-4D9A-9E7F-C78AD1418FA9}"/>
     <hyperlink ref="B38" r:id="rId208" xr:uid="{86A6B036-88EA-4716-8E85-F8D5C27399E5}"/>
     <hyperlink ref="P38" r:id="rId209" display="https://www.sec.gov/Archives/edgar/data/1512857/000090514824000687/xslForm13F_X02/primary_doc.xml" xr:uid="{B26D7B51-9986-40F5-8C9F-FEC68B715269}"/>
     <hyperlink ref="B22" r:id="rId210" xr:uid="{A9127897-D75F-4FCD-B4D5-A48BA18E3201}"/>
@@ -8922,68 +8958,68 @@
     <hyperlink ref="Q47" r:id="rId298" display="https://www.sec.gov/Archives/edgar/data/1747057/000117266124002322/xslForm13F_X02/primary_doc.xml" xr:uid="{7C6C125C-7391-415E-844A-B89AA453913D}"/>
     <hyperlink ref="R48" r:id="rId299" display="https://www.sec.gov/Archives/edgar/data/1387322/000117266124003527/xslForm13F_X02/primary_doc.xml" xr:uid="{4E0C2AA7-76C3-408C-9E0B-69FF44664D57}"/>
     <hyperlink ref="Q48" r:id="rId300" display="https://www.sec.gov/Archives/edgar/data/1387322/000138732224000004/xslForm13F_X02/primary_doc.xml" xr:uid="{011B6B5F-5865-4BBA-8289-2372CC51220A}"/>
-    <hyperlink ref="R49" r:id="rId301" display="https://www.sec.gov/Archives/edgar/data/1009258/000095015924000249/xslForm13F_X02/primary_doc.xml" xr:uid="{207F6644-0D54-407E-9FCD-AA941152BCD8}"/>
-    <hyperlink ref="Q49" r:id="rId302" display="https://www.sec.gov/Archives/edgar/data/1009258/000095015924000176/xslForm13F_X02/primary_doc.xml" xr:uid="{1E2EAF7D-A930-4B3B-B8BC-65859FC51D36}"/>
-    <hyperlink ref="R50" r:id="rId303" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957424004698/xslForm13F_X02/primary_doc.xml" xr:uid="{14EBE368-448D-4F18-A175-8DC22C34E9E7}"/>
-    <hyperlink ref="Q50" r:id="rId304" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957424003156/xslForm13F_X02/primary_doc.xml" xr:uid="{447D5F8B-79C4-48B3-8F21-FFA064B0A17D}"/>
-    <hyperlink ref="R51" r:id="rId305" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266124003539/xslForm13F_X02/primary_doc.xml" xr:uid="{FA4B05DB-81AA-4E19-9BDE-5D7AE878507B}"/>
-    <hyperlink ref="Q51" r:id="rId306" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266124002506/xslForm13F_X02/primary_doc.xml" xr:uid="{827EA756-C0E5-49D7-A4F6-E8EF5FBE9202}"/>
-    <hyperlink ref="R52" r:id="rId307" display="https://www.sec.gov/Archives/edgar/data/934639/000094787124000690/xslForm13F_X02/primary_doc.xml" xr:uid="{5CF815A6-5559-4EDA-833E-90A5B42447B6}"/>
-    <hyperlink ref="Q52" r:id="rId308" display="https://www.sec.gov/Archives/edgar/data/934639/000094787124000481/xslForm13F_X02/primary_doc.xml" xr:uid="{1144DA80-A012-449C-941A-2EB6B1DF61BE}"/>
-    <hyperlink ref="R55" r:id="rId309" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012324008753/xslForm13F_X02/primary_doc.xml" xr:uid="{43C49EA2-F799-4EFF-9529-72005064B49E}"/>
-    <hyperlink ref="Q55" r:id="rId310" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012324005626/xslForm13F_X02/primary_doc.xml" xr:uid="{D018B3CE-CC13-4D7A-A3C8-74344E1EEBE0}"/>
-    <hyperlink ref="R57" r:id="rId311" display="https://www.sec.gov/Archives/edgar/data/1319998/000101297524000330/xslForm13F_X02/primary_doc.xml" xr:uid="{B0766213-A499-42DC-A923-1E2DD4963AF8}"/>
-    <hyperlink ref="Q57" r:id="rId312" display="https://www.sec.gov/Archives/edgar/data/1319998/000101297524000225/xslForm13F_X02/primary_doc.xml" xr:uid="{E94966F1-019E-4238-A2AC-42FC2A503F52}"/>
-    <hyperlink ref="R58" r:id="rId313" display="https://www.sec.gov/Archives/edgar/data/1061768/000156761924000363/xslForm13F_X02/primary_doc.xml" xr:uid="{6C8238DE-28EC-4F2E-AB94-32FB0A061FB0}"/>
-    <hyperlink ref="Q58" r:id="rId314" display="https://www.sec.gov/Archives/edgar/data/1061768/000156761924000317/xslForm13F_X02/primary_doc.xml" xr:uid="{6542D9C5-7F31-4A28-A03D-C7AE47BCDFE4}"/>
-    <hyperlink ref="R59" r:id="rId315" display="https://www.sec.gov/Archives/edgar/data/1595082/000159508224000047/xslForm13F_X02/primary_doc.xml" xr:uid="{B06ACE8E-9710-4E91-88A6-6C67D9FFE886}"/>
-    <hyperlink ref="Q59" r:id="rId316" display="https://www.sec.gov/Archives/edgar/data/1595082/000159508224000032/xslForm13F_X02/primary_doc.xml" xr:uid="{6DE85CA7-94ED-4BCF-AAEE-BE441A132FD7}"/>
-    <hyperlink ref="R60" r:id="rId317" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297524000329/xslForm13F_X02/primary_doc.xml" xr:uid="{9F308DA5-20BD-4ACB-B608-BBBCD8F307B2}"/>
-    <hyperlink ref="Q60" r:id="rId318" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297524000218/xslForm13F_X02/primary_doc.xml" xr:uid="{9C8A5BA5-0403-4FEE-8AF0-222486610EC0}"/>
-    <hyperlink ref="R61" r:id="rId319" display="https://www.sec.gov/Archives/edgar/data/1352851/000110465924089338/xslForm13F_X02/primary_doc.xml" xr:uid="{859EE926-5F7E-4355-ACB5-3DEF3B9E6B77}"/>
-    <hyperlink ref="Q61" r:id="rId320" display="https://www.sec.gov/Archives/edgar/data/1352851/000110465924061615/xslForm13F_X02/primary_doc.xml" xr:uid="{BFA97946-69CB-4642-8D20-290708EDD539}"/>
-    <hyperlink ref="R62" r:id="rId321" display="https://www.sec.gov/Archives/edgar/data/1856083/000185608324000003/xslForm13F_X02/primary_doc.xml" xr:uid="{4F6D29E3-77B5-414C-A3AE-9090CAA7615F}"/>
-    <hyperlink ref="Q62" r:id="rId322" display="https://www.sec.gov/Archives/edgar/data/1856083/000185608324000002/xslForm13F_X02/primary_doc.xml" xr:uid="{191D46AC-51C6-4FCD-927E-84403C716A36}"/>
-    <hyperlink ref="P62" r:id="rId323" display="https://www.sec.gov/Archives/edgar/data/1856083/000185608324000001/xslForm13F_X02/primary_doc.xml" xr:uid="{9D0516F2-1F7E-4ACF-9DAE-A8696C12B258}"/>
-    <hyperlink ref="R64" r:id="rId324" display="https://www.sec.gov/Archives/edgar/data/1666335/000166633524000011/xslForm13F_X02/primary_doc.xml" xr:uid="{A8BC07D5-7D3F-4231-96DA-830ED3DCA3E2}"/>
-    <hyperlink ref="Q64" r:id="rId325" display="https://www.sec.gov/Archives/edgar/data/1666335/000166633524000008/xslForm13F_X02/primary_doc.xml" xr:uid="{DFB8487F-810A-48A1-9AC3-097192BEE32D}"/>
-    <hyperlink ref="R67" r:id="rId326" display="https://www.sec.gov/Archives/edgar/data/1443689/000144368924000012/xslForm13F_X02/primary_doc.xml" xr:uid="{66B4FDD9-F647-49D3-BD5B-AD6D1285B664}"/>
-    <hyperlink ref="Q67" r:id="rId327" display="https://www.sec.gov/Archives/edgar/data/1443689/000144368924000005/xslForm13F_X02/primary_doc.xml" xr:uid="{A8F2A4B5-023B-443A-A358-9AB6D0945F26}"/>
-    <hyperlink ref="R74" r:id="rId328" display="https://www.sec.gov/Archives/edgar/data/1290162/000095012324008706/xslForm13F_X02/primary_doc.xml" xr:uid="{5AEBD1D5-C337-449D-955C-234BC4DF2557}"/>
-    <hyperlink ref="Q74" r:id="rId329" display="https://www.sec.gov/Archives/edgar/data/1290162/000095012324005532/xslForm13F_X02/primary_doc.xml" xr:uid="{48B439C5-0B05-4A8E-9B2A-3ED8A281371F}"/>
-    <hyperlink ref="R76" r:id="rId330" display="https://www.sec.gov/Archives/edgar/data/1998597/000090266424005100/xslForm13F_X02/primary_doc.xml" xr:uid="{82A76293-0486-495C-9EBC-A6460D7D3F10}"/>
-    <hyperlink ref="Q76" r:id="rId331" display="https://www.sec.gov/Archives/edgar/data/1998597/000090266424003586/xslForm13F_X02/primary_doc.xml" xr:uid="{82316700-CD88-42C9-BBDE-F85D8E48F304}"/>
-    <hyperlink ref="R77" r:id="rId332" display="https://www.sec.gov/Archives/edgar/data/1608485/000091957424004539/xslForm13F_X02/primary_doc.xml" xr:uid="{C85C7BB6-8807-4FA6-8606-4BCE6B10A6FD}"/>
-    <hyperlink ref="Q77" r:id="rId333" display="https://www.sec.gov/Archives/edgar/data/1608485/000091957424002890/xslForm13F_X02/primary_doc.xml" xr:uid="{57E48549-351D-4871-B294-B51EAD7384A4}"/>
-    <hyperlink ref="R78" r:id="rId334" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692324000010/xslForm13F_X02/primary_doc.xml" xr:uid="{381F1CC8-2DA0-4500-843D-CBF79864963A}"/>
-    <hyperlink ref="Q78" r:id="rId335" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692324000008/xslForm13F_X02/primary_doc.xml" xr:uid="{9EAFEAFD-FBBF-48F8-8012-4BD5D5FD3E1C}"/>
-    <hyperlink ref="R79" r:id="rId336" display="https://www.sec.gov/Archives/edgar/data/1817652/000181765224000004/xslForm13F_X02/primary_doc.xml" xr:uid="{517C6364-CBED-4DDA-B6AC-E0113B993E4E}"/>
-    <hyperlink ref="Q79" r:id="rId337" display="https://www.sec.gov/Archives/edgar/data/1817652/000181765224000003/xslForm13F_X02/primary_doc.xml" xr:uid="{4CDEDDDE-7F92-4063-8C44-F119BE025583}"/>
-    <hyperlink ref="R80" r:id="rId338" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465924014706/xslForm13F_X02/primary_doc.xml" xr:uid="{1385A9AA-11EA-4110-AD65-AB8E85F329DD}"/>
-    <hyperlink ref="Q80" r:id="rId339" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465924009328/xslForm13F_X02/primary_doc.xml" xr:uid="{5A40FAC4-E535-4316-8A88-48554530AABD}"/>
-    <hyperlink ref="R82" r:id="rId340" display="https://www.sec.gov/Archives/edgar/data/1534261/000091957424004750/xslForm13F_X02/primary_doc.xml" xr:uid="{B29A2B30-D612-4093-972F-52310C3A5E79}"/>
-    <hyperlink ref="Q82" r:id="rId341" display="https://www.sec.gov/Archives/edgar/data/1534261/000091957424003198/xslForm13F_X02/primary_doc.xml" xr:uid="{E0C8D444-ABA5-492E-A820-817E70BE1B66}"/>
+    <hyperlink ref="R50" r:id="rId301" display="https://www.sec.gov/Archives/edgar/data/1009258/000095015924000249/xslForm13F_X02/primary_doc.xml" xr:uid="{207F6644-0D54-407E-9FCD-AA941152BCD8}"/>
+    <hyperlink ref="Q50" r:id="rId302" display="https://www.sec.gov/Archives/edgar/data/1009258/000095015924000176/xslForm13F_X02/primary_doc.xml" xr:uid="{1E2EAF7D-A930-4B3B-B8BC-65859FC51D36}"/>
+    <hyperlink ref="R51" r:id="rId303" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957424004698/xslForm13F_X02/primary_doc.xml" xr:uid="{14EBE368-448D-4F18-A175-8DC22C34E9E7}"/>
+    <hyperlink ref="Q51" r:id="rId304" display="https://www.sec.gov/Archives/edgar/data/1421097/000091957424003156/xslForm13F_X02/primary_doc.xml" xr:uid="{447D5F8B-79C4-48B3-8F21-FFA064B0A17D}"/>
+    <hyperlink ref="R52" r:id="rId305" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266124003539/xslForm13F_X02/primary_doc.xml" xr:uid="{FA4B05DB-81AA-4E19-9BDE-5D7AE878507B}"/>
+    <hyperlink ref="Q52" r:id="rId306" display="https://www.sec.gov/Archives/edgar/data/1055951/000117266124002506/xslForm13F_X02/primary_doc.xml" xr:uid="{827EA756-C0E5-49D7-A4F6-E8EF5FBE9202}"/>
+    <hyperlink ref="R53" r:id="rId307" display="https://www.sec.gov/Archives/edgar/data/934639/000094787124000690/xslForm13F_X02/primary_doc.xml" xr:uid="{5CF815A6-5559-4EDA-833E-90A5B42447B6}"/>
+    <hyperlink ref="Q53" r:id="rId308" display="https://www.sec.gov/Archives/edgar/data/934639/000094787124000481/xslForm13F_X02/primary_doc.xml" xr:uid="{1144DA80-A012-449C-941A-2EB6B1DF61BE}"/>
+    <hyperlink ref="R56" r:id="rId309" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012324008753/xslForm13F_X02/primary_doc.xml" xr:uid="{43C49EA2-F799-4EFF-9529-72005064B49E}"/>
+    <hyperlink ref="Q56" r:id="rId310" display="https://www.sec.gov/Archives/edgar/data/1054587/000095012324005626/xslForm13F_X02/primary_doc.xml" xr:uid="{D018B3CE-CC13-4D7A-A3C8-74344E1EEBE0}"/>
+    <hyperlink ref="R58" r:id="rId311" display="https://www.sec.gov/Archives/edgar/data/1319998/000101297524000330/xslForm13F_X02/primary_doc.xml" xr:uid="{B0766213-A499-42DC-A923-1E2DD4963AF8}"/>
+    <hyperlink ref="Q58" r:id="rId312" display="https://www.sec.gov/Archives/edgar/data/1319998/000101297524000225/xslForm13F_X02/primary_doc.xml" xr:uid="{E94966F1-019E-4238-A2AC-42FC2A503F52}"/>
+    <hyperlink ref="R59" r:id="rId313" display="https://www.sec.gov/Archives/edgar/data/1061768/000156761924000363/xslForm13F_X02/primary_doc.xml" xr:uid="{6C8238DE-28EC-4F2E-AB94-32FB0A061FB0}"/>
+    <hyperlink ref="Q59" r:id="rId314" display="https://www.sec.gov/Archives/edgar/data/1061768/000156761924000317/xslForm13F_X02/primary_doc.xml" xr:uid="{6542D9C5-7F31-4A28-A03D-C7AE47BCDFE4}"/>
+    <hyperlink ref="R60" r:id="rId315" display="https://www.sec.gov/Archives/edgar/data/1595082/000159508224000047/xslForm13F_X02/primary_doc.xml" xr:uid="{B06ACE8E-9710-4E91-88A6-6C67D9FFE886}"/>
+    <hyperlink ref="Q60" r:id="rId316" display="https://www.sec.gov/Archives/edgar/data/1595082/000159508224000032/xslForm13F_X02/primary_doc.xml" xr:uid="{6DE85CA7-94ED-4BCF-AAEE-BE441A132FD7}"/>
+    <hyperlink ref="R61" r:id="rId317" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297524000329/xslForm13F_X02/primary_doc.xml" xr:uid="{9F308DA5-20BD-4ACB-B608-BBBCD8F307B2}"/>
+    <hyperlink ref="Q61" r:id="rId318" display="https://www.sec.gov/Archives/edgar/data/1224962/000101297524000218/xslForm13F_X02/primary_doc.xml" xr:uid="{9C8A5BA5-0403-4FEE-8AF0-222486610EC0}"/>
+    <hyperlink ref="R62" r:id="rId319" display="https://www.sec.gov/Archives/edgar/data/1352851/000110465924089338/xslForm13F_X02/primary_doc.xml" xr:uid="{859EE926-5F7E-4355-ACB5-3DEF3B9E6B77}"/>
+    <hyperlink ref="Q62" r:id="rId320" display="https://www.sec.gov/Archives/edgar/data/1352851/000110465924061615/xslForm13F_X02/primary_doc.xml" xr:uid="{BFA97946-69CB-4642-8D20-290708EDD539}"/>
+    <hyperlink ref="R63" r:id="rId321" display="https://www.sec.gov/Archives/edgar/data/1856083/000185608324000003/xslForm13F_X02/primary_doc.xml" xr:uid="{4F6D29E3-77B5-414C-A3AE-9090CAA7615F}"/>
+    <hyperlink ref="Q63" r:id="rId322" display="https://www.sec.gov/Archives/edgar/data/1856083/000185608324000002/xslForm13F_X02/primary_doc.xml" xr:uid="{191D46AC-51C6-4FCD-927E-84403C716A36}"/>
+    <hyperlink ref="P63" r:id="rId323" display="https://www.sec.gov/Archives/edgar/data/1856083/000185608324000001/xslForm13F_X02/primary_doc.xml" xr:uid="{9D0516F2-1F7E-4ACF-9DAE-A8696C12B258}"/>
+    <hyperlink ref="R65" r:id="rId324" display="https://www.sec.gov/Archives/edgar/data/1666335/000166633524000011/xslForm13F_X02/primary_doc.xml" xr:uid="{A8BC07D5-7D3F-4231-96DA-830ED3DCA3E2}"/>
+    <hyperlink ref="Q65" r:id="rId325" display="https://www.sec.gov/Archives/edgar/data/1666335/000166633524000008/xslForm13F_X02/primary_doc.xml" xr:uid="{DFB8487F-810A-48A1-9AC3-097192BEE32D}"/>
+    <hyperlink ref="R68" r:id="rId326" display="https://www.sec.gov/Archives/edgar/data/1443689/000144368924000012/xslForm13F_X02/primary_doc.xml" xr:uid="{66B4FDD9-F647-49D3-BD5B-AD6D1285B664}"/>
+    <hyperlink ref="Q68" r:id="rId327" display="https://www.sec.gov/Archives/edgar/data/1443689/000144368924000005/xslForm13F_X02/primary_doc.xml" xr:uid="{A8F2A4B5-023B-443A-A358-9AB6D0945F26}"/>
+    <hyperlink ref="R75" r:id="rId328" display="https://www.sec.gov/Archives/edgar/data/1290162/000095012324008706/xslForm13F_X02/primary_doc.xml" xr:uid="{5AEBD1D5-C337-449D-955C-234BC4DF2557}"/>
+    <hyperlink ref="Q75" r:id="rId329" display="https://www.sec.gov/Archives/edgar/data/1290162/000095012324005532/xslForm13F_X02/primary_doc.xml" xr:uid="{48B439C5-0B05-4A8E-9B2A-3ED8A281371F}"/>
+    <hyperlink ref="R77" r:id="rId330" display="https://www.sec.gov/Archives/edgar/data/1998597/000090266424005100/xslForm13F_X02/primary_doc.xml" xr:uid="{82A76293-0486-495C-9EBC-A6460D7D3F10}"/>
+    <hyperlink ref="Q77" r:id="rId331" display="https://www.sec.gov/Archives/edgar/data/1998597/000090266424003586/xslForm13F_X02/primary_doc.xml" xr:uid="{82316700-CD88-42C9-BBDE-F85D8E48F304}"/>
+    <hyperlink ref="R78" r:id="rId332" display="https://www.sec.gov/Archives/edgar/data/1608485/000091957424004539/xslForm13F_X02/primary_doc.xml" xr:uid="{C85C7BB6-8807-4FA6-8606-4BCE6B10A6FD}"/>
+    <hyperlink ref="Q78" r:id="rId333" display="https://www.sec.gov/Archives/edgar/data/1608485/000091957424002890/xslForm13F_X02/primary_doc.xml" xr:uid="{57E48549-351D-4871-B294-B51EAD7384A4}"/>
+    <hyperlink ref="R79" r:id="rId334" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692324000010/xslForm13F_X02/primary_doc.xml" xr:uid="{381F1CC8-2DA0-4500-843D-CBF79864963A}"/>
+    <hyperlink ref="Q79" r:id="rId335" display="https://www.sec.gov/Archives/edgar/data/1306923/000130692324000008/xslForm13F_X02/primary_doc.xml" xr:uid="{9EAFEAFD-FBBF-48F8-8012-4BD5D5FD3E1C}"/>
+    <hyperlink ref="R80" r:id="rId336" display="https://www.sec.gov/Archives/edgar/data/1817652/000181765224000004/xslForm13F_X02/primary_doc.xml" xr:uid="{517C6364-CBED-4DDA-B6AC-E0113B993E4E}"/>
+    <hyperlink ref="Q80" r:id="rId337" display="https://www.sec.gov/Archives/edgar/data/1817652/000181765224000003/xslForm13F_X02/primary_doc.xml" xr:uid="{4CDEDDDE-7F92-4063-8C44-F119BE025583}"/>
+    <hyperlink ref="R81" r:id="rId338" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465924014706/xslForm13F_X02/primary_doc.xml" xr:uid="{1385A9AA-11EA-4110-AD65-AB8E85F329DD}"/>
+    <hyperlink ref="Q81" r:id="rId339" display="https://www.sec.gov/Archives/edgar/data/1232621/000121465924009328/xslForm13F_X02/primary_doc.xml" xr:uid="{5A40FAC4-E535-4316-8A88-48554530AABD}"/>
+    <hyperlink ref="R83" r:id="rId340" display="https://www.sec.gov/Archives/edgar/data/1534261/000091957424004750/xslForm13F_X02/primary_doc.xml" xr:uid="{B29A2B30-D612-4093-972F-52310C3A5E79}"/>
+    <hyperlink ref="Q83" r:id="rId341" display="https://www.sec.gov/Archives/edgar/data/1534261/000091957424003198/xslForm13F_X02/primary_doc.xml" xr:uid="{E0C8D444-ABA5-492E-A820-817E70BE1B66}"/>
     <hyperlink ref="R38" r:id="rId342" display="https://www.sec.gov/Archives/edgar/data/1512857/000090514824002211/xslForm13F_X02/primary_doc.xml" xr:uid="{1761334C-56A2-4846-8F57-4A9DD09F5ECB}"/>
     <hyperlink ref="Q38" r:id="rId343" display="https://www.sec.gov/Archives/edgar/data/1512857/000090514824001428/xslForm13F_X02/primary_doc.xml" xr:uid="{7E1A6809-D273-45E4-983B-D2CB04D5C260}"/>
-    <hyperlink ref="R86" r:id="rId344" display="https://www.sec.gov/Archives/edgar/data/1279150/000199937124010097/xslForm13F_X02/primary_doc.xml" xr:uid="{ADFD8AB4-808C-468F-85A1-2E21CDB320FE}"/>
-    <hyperlink ref="Q86" r:id="rId345" display="https://www.sec.gov/Archives/edgar/data/1279150/000199937124006136/xslForm13F_X02/primary_doc.xml" xr:uid="{88E53C5B-5DD6-4C5E-9460-AA69DA132B22}"/>
+    <hyperlink ref="R87" r:id="rId344" display="https://www.sec.gov/Archives/edgar/data/1279150/000199937124010097/xslForm13F_X02/primary_doc.xml" xr:uid="{ADFD8AB4-808C-468F-85A1-2E21CDB320FE}"/>
+    <hyperlink ref="Q87" r:id="rId345" display="https://www.sec.gov/Archives/edgar/data/1279150/000199937124006136/xslForm13F_X02/primary_doc.xml" xr:uid="{88E53C5B-5DD6-4C5E-9460-AA69DA132B22}"/>
     <hyperlink ref="B32" r:id="rId346" xr:uid="{1E6E3C8D-5839-4837-95D4-93A295AE3A18}"/>
     <hyperlink ref="R32" r:id="rId347" display="https://www.sec.gov/Archives/edgar/data/1541617/000154161724000007/xslForm13F_X02/primary_doc.xml" xr:uid="{481D1746-D6ED-474F-8BE4-34D4D4759CFF}"/>
     <hyperlink ref="Q32" r:id="rId348" display="https://www.sec.gov/Archives/edgar/data/1541617/000154161724000006/xslForm13F_X02/primary_doc.xml" xr:uid="{D3FFF611-340F-47FC-9BA1-F8B336CFBF18}"/>
     <hyperlink ref="P32" r:id="rId349" display="https://www.sec.gov/Archives/edgar/data/1541617/000154161724000004/xslForm13F_X02/primary_doc.xml" xr:uid="{06EDB189-B640-4942-917A-7DB590381FB8}"/>
-    <hyperlink ref="B81" r:id="rId350" xr:uid="{83904953-99D5-46A7-AB9A-51816F9E05BD}"/>
-    <hyperlink ref="R81" r:id="rId351" display="https://www.sec.gov/Archives/edgar/data/1583977/000158397724000003/xslForm13F_X02/primary_doc.xml" xr:uid="{59C53B2D-3983-4FAF-B152-B54147E1CDCD}"/>
-    <hyperlink ref="Q81" r:id="rId352" display="https://www.sec.gov/Archives/edgar/data/1583977/000158397724000002/xslForm13F_X02/primary_doc.xml" xr:uid="{CD57EC89-86CA-48E0-96C9-3C439F58F2B5}"/>
-    <hyperlink ref="P81" r:id="rId353" display="https://www.sec.gov/Archives/edgar/data/1583977/000158397724000001/xslForm13F_X02/primary_doc.xml" xr:uid="{B9C7A2BA-FBD9-4FAF-A09E-1C8DE7F140AB}"/>
+    <hyperlink ref="B82" r:id="rId350" xr:uid="{83904953-99D5-46A7-AB9A-51816F9E05BD}"/>
+    <hyperlink ref="R82" r:id="rId351" display="https://www.sec.gov/Archives/edgar/data/1583977/000158397724000003/xslForm13F_X02/primary_doc.xml" xr:uid="{59C53B2D-3983-4FAF-B152-B54147E1CDCD}"/>
+    <hyperlink ref="Q82" r:id="rId352" display="https://www.sec.gov/Archives/edgar/data/1583977/000158397724000002/xslForm13F_X02/primary_doc.xml" xr:uid="{CD57EC89-86CA-48E0-96C9-3C439F58F2B5}"/>
+    <hyperlink ref="P82" r:id="rId353" display="https://www.sec.gov/Archives/edgar/data/1583977/000158397724000001/xslForm13F_X02/primary_doc.xml" xr:uid="{B9C7A2BA-FBD9-4FAF-A09E-1C8DE7F140AB}"/>
     <hyperlink ref="O10" r:id="rId354" display="https://www.sec.gov/Archives/edgar/data/1167557/000108514622004118/xslForm13F_X01/primary_doc.xml" xr:uid="{38CC0D06-6D9F-4333-9097-760F1202AD4E}"/>
     <hyperlink ref="N10" r:id="rId355" display="https://www.sec.gov/Archives/edgar/data/1167557/000108514623003416/xslForm13F_X02/primary_doc.xml" xr:uid="{4FE4B2E7-AFA1-421D-AA3D-32F9082ED7E7}"/>
     <hyperlink ref="M10" r:id="rId356" display="https://www.sec.gov/Archives/edgar/data/1167557/000108514624002596/xslForm13F_X02/primary_doc.xml" xr:uid="{15E646F2-7AF3-41C2-97AE-1C1B68785302}"/>
     <hyperlink ref="B31" r:id="rId357" xr:uid="{E2FE8C3B-BF8D-41A4-9A6B-12A304C5BB4E}"/>
     <hyperlink ref="R31" r:id="rId358" display="https://www.sec.gov/Archives/edgar/data/1425851/000114036124035138/xslForm13F_X02/primary_doc.xml" xr:uid="{805AD2FB-D592-4CE1-88BF-79840EBDAA05}"/>
-    <hyperlink ref="B84" r:id="rId359" xr:uid="{44690143-8DF9-41FA-BD6E-B315C63FFF23}"/>
-    <hyperlink ref="R84" r:id="rId360" display="https://www.sec.gov/Archives/edgar/data/1484972/000108514624003962/xslForm13F_X02/primary_doc.xml" xr:uid="{4E414D99-59A1-45EA-9098-BA19D7E99D6E}"/>
-    <hyperlink ref="B70" r:id="rId361" xr:uid="{F44B669C-37C6-4B65-97AF-E11A600F0DE2}"/>
-    <hyperlink ref="R70" r:id="rId362" display="https://www.sec.gov/Archives/edgar/data/872573/000087257324000019/xslForm13F_X02/primary_doc.xml" xr:uid="{72759C36-E206-4B33-8190-3995F18A0CD4}"/>
+    <hyperlink ref="B85" r:id="rId359" xr:uid="{44690143-8DF9-41FA-BD6E-B315C63FFF23}"/>
+    <hyperlink ref="R85" r:id="rId360" display="https://www.sec.gov/Archives/edgar/data/1484972/000108514624003962/xslForm13F_X02/primary_doc.xml" xr:uid="{4E414D99-59A1-45EA-9098-BA19D7E99D6E}"/>
+    <hyperlink ref="B71" r:id="rId361" xr:uid="{F44B669C-37C6-4B65-97AF-E11A600F0DE2}"/>
+    <hyperlink ref="R71" r:id="rId362" display="https://www.sec.gov/Archives/edgar/data/872573/000087257324000019/xslForm13F_X02/primary_doc.xml" xr:uid="{72759C36-E206-4B33-8190-3995F18A0CD4}"/>
     <hyperlink ref="B45" r:id="rId363" xr:uid="{5077FC4B-31AF-4A7A-A8B4-84F14707CE77}"/>
     <hyperlink ref="R45" r:id="rId364" display="https://www.sec.gov/Archives/edgar/data/1706766/000170676624000005/xslForm13F_X02/primary_doc.xml" xr:uid="{C4F52B96-9054-4E80-9FD3-F7AB0076EC4F}"/>
     <hyperlink ref="B30" r:id="rId365" xr:uid="{A67231F9-2C7E-4B9C-ABD0-4FD0F2449A48}"/>
@@ -8994,60 +9030,64 @@
     <hyperlink ref="R12" r:id="rId370" display="https://www.sec.gov/Archives/edgar/data/1729829/000172982924000011/xslForm13F_X02/primary_doc.xml" xr:uid="{5BF9E6D6-92E9-410B-B94C-CF38C0132D7E}"/>
     <hyperlink ref="Q12" r:id="rId371" display="https://www.sec.gov/Archives/edgar/data/1729829/000172982924000009/xslForm13F_X02/primary_doc.xml" xr:uid="{950E9310-7859-469C-9CC5-AB6180940F72}"/>
     <hyperlink ref="P12" r:id="rId372" display="https://www.sec.gov/Archives/edgar/data/1729829/000172982924000003/xslForm13F_X02/primary_doc.xml" xr:uid="{7C510404-0EA5-49B4-9D8E-42DA7C328856}"/>
-    <hyperlink ref="B56" r:id="rId373" xr:uid="{6AD05462-74B2-4204-99E0-8FB5FA073108}"/>
-    <hyperlink ref="R56" r:id="rId374" display="https://www.sec.gov/Archives/edgar/data/1509842/000095012324008739/xslForm13F_X02/primary_doc.xml" xr:uid="{9EB7194B-8466-4DE0-B2D0-57A49C5B2060}"/>
-    <hyperlink ref="B66" r:id="rId375" xr:uid="{49A94717-D9CE-4E51-9173-86A9C3169185}"/>
-    <hyperlink ref="R66" r:id="rId376" display="https://www.sec.gov/Archives/edgar/data/1595725/000117266124003467/xslForm13F_X02/primary_doc.xml" xr:uid="{92E4CA42-890B-42B5-9C21-995F5C803B4D}"/>
-    <hyperlink ref="Q66" r:id="rId377" display="https://www.sec.gov/Archives/edgar/data/1595725/000117266124002385/xslForm13F_X02/primary_doc.xml" xr:uid="{DB6CE2BA-40B7-4F26-9A16-1A5E952A0956}"/>
-    <hyperlink ref="P66" r:id="rId378" display="https://www.sec.gov/Archives/edgar/data/1595725/000117266124001078/xslForm13F_X02/primary_doc.xml" xr:uid="{CFBBD04A-0F9C-4D46-8F26-7F1FC37324AE}"/>
-    <hyperlink ref="R75" r:id="rId379" display="https://www.sec.gov/Archives/edgar/data/1803916/000180391624000004/xslForm13F_X02/primary_doc.xml" xr:uid="{54DFF6A0-5D1D-4547-A1D3-4D4F4DD5FD94}"/>
-    <hyperlink ref="R73" r:id="rId380" display="https://www.sec.gov/Archives/edgar/data/1489933/000117266124003549/xslForm13F_X02/primary_doc.xml" xr:uid="{CA3501A4-D14E-4403-A16A-759949B1DAEF}"/>
-    <hyperlink ref="R87" r:id="rId381" display="https://www.sec.gov/Archives/edgar/data/1940272/000194026724000001/xslForm13F_X02/primary_doc.xml" xr:uid="{1F11647F-8D10-4578-8333-3CAF131B7591}"/>
-    <hyperlink ref="R65" r:id="rId382" display="https://www.sec.gov/Archives/edgar/data/936944/000093694424000006/xslForm13F_X02/primary_doc.xml" xr:uid="{7CA62473-1D9B-4F28-B6D0-BB90203E51EB}"/>
-    <hyperlink ref="B53" r:id="rId383" xr:uid="{C1C4A467-8642-4EBF-B0D6-3E19614B4959}"/>
-    <hyperlink ref="R53" r:id="rId384" display="https://www.sec.gov/Archives/edgar/data/1831577/000166773124000469/xslForm13F_X02/primary_doc.xml" xr:uid="{72562425-34DE-43D3-BD84-A4122847AA65}"/>
-    <hyperlink ref="Q53" r:id="rId385" display="https://www.sec.gov/Archives/edgar/data/1831577/000166773124000224/xslForm13F_X02/primary_doc.xml" xr:uid="{49921FB6-5B6A-4F34-806C-4A5A87A96628}"/>
-    <hyperlink ref="P53" r:id="rId386" display="https://www.sec.gov/Archives/edgar/data/1831577/000166773124000065/xslForm13F_X02/primary_doc.xml" xr:uid="{D8198C1F-89E2-47B6-BB90-4900860F390D}"/>
-    <hyperlink ref="B88" r:id="rId387" xr:uid="{789256CA-C9E5-4BB9-9B1A-834D37A1C8DF}"/>
-    <hyperlink ref="R88" r:id="rId388" display="https://www.sec.gov/Archives/edgar/data/1595521/000159552124000005/xslForm13F_X02/primary_doc.xml" xr:uid="{60A788B3-0D56-4EBE-806D-350CCFE02AEB}"/>
-    <hyperlink ref="Q88" r:id="rId389" display="https://www.sec.gov/Archives/edgar/data/1595521/000159552124000004/xslForm13F_X02/primary_doc.xml" xr:uid="{DA17B8C2-43B4-44FC-BDDC-60A44D15421B}"/>
-    <hyperlink ref="P88" r:id="rId390" display="https://www.sec.gov/Archives/edgar/data/1595521/000159552124000002/xslForm13F_X02/primary_doc.xml" xr:uid="{92B3E41C-3585-4797-A1F9-4F3C7C3A191D}"/>
+    <hyperlink ref="B57" r:id="rId373" xr:uid="{6AD05462-74B2-4204-99E0-8FB5FA073108}"/>
+    <hyperlink ref="R57" r:id="rId374" display="https://www.sec.gov/Archives/edgar/data/1509842/000095012324008739/xslForm13F_X02/primary_doc.xml" xr:uid="{9EB7194B-8466-4DE0-B2D0-57A49C5B2060}"/>
+    <hyperlink ref="B67" r:id="rId375" xr:uid="{49A94717-D9CE-4E51-9173-86A9C3169185}"/>
+    <hyperlink ref="R67" r:id="rId376" display="https://www.sec.gov/Archives/edgar/data/1595725/000117266124003467/xslForm13F_X02/primary_doc.xml" xr:uid="{92E4CA42-890B-42B5-9C21-995F5C803B4D}"/>
+    <hyperlink ref="Q67" r:id="rId377" display="https://www.sec.gov/Archives/edgar/data/1595725/000117266124002385/xslForm13F_X02/primary_doc.xml" xr:uid="{DB6CE2BA-40B7-4F26-9A16-1A5E952A0956}"/>
+    <hyperlink ref="P67" r:id="rId378" display="https://www.sec.gov/Archives/edgar/data/1595725/000117266124001078/xslForm13F_X02/primary_doc.xml" xr:uid="{CFBBD04A-0F9C-4D46-8F26-7F1FC37324AE}"/>
+    <hyperlink ref="R76" r:id="rId379" display="https://www.sec.gov/Archives/edgar/data/1803916/000180391624000004/xslForm13F_X02/primary_doc.xml" xr:uid="{54DFF6A0-5D1D-4547-A1D3-4D4F4DD5FD94}"/>
+    <hyperlink ref="R74" r:id="rId380" display="https://www.sec.gov/Archives/edgar/data/1489933/000117266124003549/xslForm13F_X02/primary_doc.xml" xr:uid="{CA3501A4-D14E-4403-A16A-759949B1DAEF}"/>
+    <hyperlink ref="R88" r:id="rId381" display="https://www.sec.gov/Archives/edgar/data/1940272/000194026724000001/xslForm13F_X02/primary_doc.xml" xr:uid="{1F11647F-8D10-4578-8333-3CAF131B7591}"/>
+    <hyperlink ref="R66" r:id="rId382" display="https://www.sec.gov/Archives/edgar/data/936944/000093694424000006/xslForm13F_X02/primary_doc.xml" xr:uid="{7CA62473-1D9B-4F28-B6D0-BB90203E51EB}"/>
+    <hyperlink ref="B54" r:id="rId383" xr:uid="{C1C4A467-8642-4EBF-B0D6-3E19614B4959}"/>
+    <hyperlink ref="R54" r:id="rId384" display="https://www.sec.gov/Archives/edgar/data/1831577/000166773124000469/xslForm13F_X02/primary_doc.xml" xr:uid="{72562425-34DE-43D3-BD84-A4122847AA65}"/>
+    <hyperlink ref="Q54" r:id="rId385" display="https://www.sec.gov/Archives/edgar/data/1831577/000166773124000224/xslForm13F_X02/primary_doc.xml" xr:uid="{49921FB6-5B6A-4F34-806C-4A5A87A96628}"/>
+    <hyperlink ref="P54" r:id="rId386" display="https://www.sec.gov/Archives/edgar/data/1831577/000166773124000065/xslForm13F_X02/primary_doc.xml" xr:uid="{D8198C1F-89E2-47B6-BB90-4900860F390D}"/>
+    <hyperlink ref="B89" r:id="rId387" xr:uid="{789256CA-C9E5-4BB9-9B1A-834D37A1C8DF}"/>
+    <hyperlink ref="R89" r:id="rId388" display="https://www.sec.gov/Archives/edgar/data/1595521/000159552124000005/xslForm13F_X02/primary_doc.xml" xr:uid="{60A788B3-0D56-4EBE-806D-350CCFE02AEB}"/>
+    <hyperlink ref="Q89" r:id="rId389" display="https://www.sec.gov/Archives/edgar/data/1595521/000159552124000004/xslForm13F_X02/primary_doc.xml" xr:uid="{DA17B8C2-43B4-44FC-BDDC-60A44D15421B}"/>
+    <hyperlink ref="P89" r:id="rId390" display="https://www.sec.gov/Archives/edgar/data/1595521/000159552124000002/xslForm13F_X02/primary_doc.xml" xr:uid="{92B3E41C-3585-4797-A1F9-4F3C7C3A191D}"/>
     <hyperlink ref="B36" r:id="rId391" xr:uid="{528F9214-24B9-4A84-AD82-C9F8CFBC0326}"/>
     <hyperlink ref="R36" r:id="rId392" display="https://www.sec.gov/Archives/edgar/data/1453072/000117266124003532/xslForm13F_X02/primary_doc.xml" xr:uid="{5CF48255-0BA9-419F-A53C-2E23F2152EAE}"/>
     <hyperlink ref="Q36" r:id="rId393" display="https://www.sec.gov/Archives/edgar/data/1453072/000117266124002473/xslForm13F_X02/primary_doc.xml" xr:uid="{BBFC3495-8433-4D80-9EB6-F2D3566343BE}"/>
     <hyperlink ref="P36" r:id="rId394" display="https://www.sec.gov/Archives/edgar/data/1453072/000117266124001424/xslForm13F_X02/primary_doc.xml" xr:uid="{8D03C58C-55E2-4F4C-8685-99BFF041BD82}"/>
-    <hyperlink ref="B63" r:id="rId395" xr:uid="{A56C166E-61BD-44BF-B453-216E20027DDA}"/>
-    <hyperlink ref="R63" r:id="rId396" display="https://www.sec.gov/Archives/edgar/data/1418814/000141881224000017/xslForm13F_X02/primary_doc.xml" xr:uid="{E1F9F6DF-A92E-4081-9C02-D1312B0BBF30}"/>
-    <hyperlink ref="Q63" r:id="rId397" display="https://www.sec.gov/Archives/edgar/data/1418814/000141881224000011/xslForm13F_X02/primary_doc.xml" xr:uid="{AAA28E5D-A13B-4A4E-A93F-9BF55DC613C9}"/>
-    <hyperlink ref="P63" r:id="rId398" display="https://www.sec.gov/Archives/edgar/data/1418814/000141881224000003/xslForm13F_X02/primary_doc.xml" xr:uid="{A5713FB9-5464-46C8-89DF-2ED3759C857D}"/>
-    <hyperlink ref="B68" r:id="rId399" xr:uid="{1C417AD9-1E81-4F7D-B5A2-DB13C3E4F1C4}"/>
-    <hyperlink ref="R68" r:id="rId400" display="https://www.sec.gov/Archives/edgar/data/1444043/000165495424010537/xslForm13F_X02/primary_doc.xml" xr:uid="{DF937787-5B9C-4B35-855E-696EB50976C3}"/>
-    <hyperlink ref="Q68" r:id="rId401" display="https://www.sec.gov/Archives/edgar/data/1444043/000165495424006308/xslForm13F_X02/primary_doc.xml" xr:uid="{FA2FACBA-FE30-402F-844A-A11129D10883}"/>
-    <hyperlink ref="P68" r:id="rId402" display="https://www.sec.gov/Archives/edgar/data/1444043/000165495424001698/xslForm13F_X02/primary_doc.xml" xr:uid="{1B276C68-A159-4013-B69D-5370AE435C70}"/>
-    <hyperlink ref="B83" r:id="rId403" xr:uid="{1ED90491-9D1C-4DB3-88F0-820279C7D047}"/>
-    <hyperlink ref="R83" r:id="rId404" display="https://www.sec.gov/Archives/edgar/data/1632715/000117266124003374/xslForm13F_X02/primary_doc.xml" xr:uid="{EE7888E6-82F5-4616-9D8C-7D4D6C32FE4C}"/>
-    <hyperlink ref="Q83" r:id="rId405" display="https://www.sec.gov/Archives/edgar/data/1632715/000117266124002394/xslForm13F_X02/primary_doc.xml" xr:uid="{996F651D-D40F-4F6D-BBA0-6B79E8A756BF}"/>
-    <hyperlink ref="P83" r:id="rId406" display="https://www.sec.gov/Archives/edgar/data/1632715/000117266124000834/xslForm13F_X02/primary_doc.xml" xr:uid="{C9CD2DAA-9CB1-4028-AB58-67AE0A26C57B}"/>
-    <hyperlink ref="B54" r:id="rId407" xr:uid="{3BCAC531-3A14-469D-AA7C-72A364ACD2A5}"/>
-    <hyperlink ref="R54" r:id="rId408" display="https://www.sec.gov/Archives/edgar/data/1138995/000090514824002216/xslForm13F_X02/primary_doc.xml" xr:uid="{282B176B-230E-40FF-9C80-2D3B7EA129F2}"/>
-    <hyperlink ref="B71" r:id="rId409" xr:uid="{33F3BC97-083C-488A-A59D-0353F323F258}"/>
-    <hyperlink ref="R71" r:id="rId410" display="https://www.sec.gov/Archives/edgar/data/1512173/000091957424004559/xslForm13F_X02/primary_doc.xml" xr:uid="{2C54D3C6-DC13-470A-A67F-7BCA5D467B59}"/>
-    <hyperlink ref="B85" r:id="rId411" xr:uid="{0C6F64D3-5EFE-48D6-B0FC-156F7712F05B}"/>
-    <hyperlink ref="R85" r:id="rId412" display="https://www.sec.gov/Archives/edgar/data/1389507/000091957424004460/xslForm13F_X02/primary_doc.xml" xr:uid="{1D009CEB-3503-4121-98B9-2E845C2E5B39}"/>
-    <hyperlink ref="B69" r:id="rId413" xr:uid="{7EB1C527-4826-4856-9C5B-3CD860C7BC5C}"/>
-    <hyperlink ref="R69" r:id="rId414" display="https://www.sec.gov/Archives/edgar/data/1920938/000142050624001566/xslForm13F_X02/primary_doc.xml" xr:uid="{A19E1E20-A71C-428D-906A-837FE3391874}"/>
-    <hyperlink ref="Q69" r:id="rId415" display="https://www.sec.gov/Archives/edgar/data/1920938/000192093824000004/xslForm13F_X02/primary_doc.xml" xr:uid="{D136F781-E058-43AE-BF4A-327D36ECCE72}"/>
-    <hyperlink ref="P69" r:id="rId416" display="https://www.sec.gov/Archives/edgar/data/1920938/000142050624000478/xslForm13F_X02/primary_doc.xml" xr:uid="{CD16B160-C0FF-4B09-BDE9-92934FBD7269}"/>
+    <hyperlink ref="B64" r:id="rId395" xr:uid="{A56C166E-61BD-44BF-B453-216E20027DDA}"/>
+    <hyperlink ref="R64" r:id="rId396" display="https://www.sec.gov/Archives/edgar/data/1418814/000141881224000017/xslForm13F_X02/primary_doc.xml" xr:uid="{E1F9F6DF-A92E-4081-9C02-D1312B0BBF30}"/>
+    <hyperlink ref="Q64" r:id="rId397" display="https://www.sec.gov/Archives/edgar/data/1418814/000141881224000011/xslForm13F_X02/primary_doc.xml" xr:uid="{AAA28E5D-A13B-4A4E-A93F-9BF55DC613C9}"/>
+    <hyperlink ref="P64" r:id="rId398" display="https://www.sec.gov/Archives/edgar/data/1418814/000141881224000003/xslForm13F_X02/primary_doc.xml" xr:uid="{A5713FB9-5464-46C8-89DF-2ED3759C857D}"/>
+    <hyperlink ref="B69" r:id="rId399" xr:uid="{1C417AD9-1E81-4F7D-B5A2-DB13C3E4F1C4}"/>
+    <hyperlink ref="R69" r:id="rId400" display="https://www.sec.gov/Archives/edgar/data/1444043/000165495424010537/xslForm13F_X02/primary_doc.xml" xr:uid="{DF937787-5B9C-4B35-855E-696EB50976C3}"/>
+    <hyperlink ref="Q69" r:id="rId401" display="https://www.sec.gov/Archives/edgar/data/1444043/000165495424006308/xslForm13F_X02/primary_doc.xml" xr:uid="{FA2FACBA-FE30-402F-844A-A11129D10883}"/>
+    <hyperlink ref="P69" r:id="rId402" display="https://www.sec.gov/Archives/edgar/data/1444043/000165495424001698/xslForm13F_X02/primary_doc.xml" xr:uid="{1B276C68-A159-4013-B69D-5370AE435C70}"/>
+    <hyperlink ref="B84" r:id="rId403" xr:uid="{1ED90491-9D1C-4DB3-88F0-820279C7D047}"/>
+    <hyperlink ref="R84" r:id="rId404" display="https://www.sec.gov/Archives/edgar/data/1632715/000117266124003374/xslForm13F_X02/primary_doc.xml" xr:uid="{EE7888E6-82F5-4616-9D8C-7D4D6C32FE4C}"/>
+    <hyperlink ref="Q84" r:id="rId405" display="https://www.sec.gov/Archives/edgar/data/1632715/000117266124002394/xslForm13F_X02/primary_doc.xml" xr:uid="{996F651D-D40F-4F6D-BBA0-6B79E8A756BF}"/>
+    <hyperlink ref="P84" r:id="rId406" display="https://www.sec.gov/Archives/edgar/data/1632715/000117266124000834/xslForm13F_X02/primary_doc.xml" xr:uid="{C9CD2DAA-9CB1-4028-AB58-67AE0A26C57B}"/>
+    <hyperlink ref="B55" r:id="rId407" xr:uid="{3BCAC531-3A14-469D-AA7C-72A364ACD2A5}"/>
+    <hyperlink ref="R55" r:id="rId408" display="https://www.sec.gov/Archives/edgar/data/1138995/000090514824002216/xslForm13F_X02/primary_doc.xml" xr:uid="{282B176B-230E-40FF-9C80-2D3B7EA129F2}"/>
+    <hyperlink ref="B72" r:id="rId409" xr:uid="{33F3BC97-083C-488A-A59D-0353F323F258}"/>
+    <hyperlink ref="R72" r:id="rId410" display="https://www.sec.gov/Archives/edgar/data/1512173/000091957424004559/xslForm13F_X02/primary_doc.xml" xr:uid="{2C54D3C6-DC13-470A-A67F-7BCA5D467B59}"/>
+    <hyperlink ref="B86" r:id="rId411" xr:uid="{0C6F64D3-5EFE-48D6-B0FC-156F7712F05B}"/>
+    <hyperlink ref="R86" r:id="rId412" display="https://www.sec.gov/Archives/edgar/data/1389507/000091957424004460/xslForm13F_X02/primary_doc.xml" xr:uid="{1D009CEB-3503-4121-98B9-2E845C2E5B39}"/>
+    <hyperlink ref="B70" r:id="rId413" xr:uid="{7EB1C527-4826-4856-9C5B-3CD860C7BC5C}"/>
+    <hyperlink ref="R70" r:id="rId414" display="https://www.sec.gov/Archives/edgar/data/1920938/000142050624001566/xslForm13F_X02/primary_doc.xml" xr:uid="{A19E1E20-A71C-428D-906A-837FE3391874}"/>
+    <hyperlink ref="Q70" r:id="rId415" display="https://www.sec.gov/Archives/edgar/data/1920938/000192093824000004/xslForm13F_X02/primary_doc.xml" xr:uid="{D136F781-E058-43AE-BF4A-327D36ECCE72}"/>
+    <hyperlink ref="P70" r:id="rId416" display="https://www.sec.gov/Archives/edgar/data/1920938/000142050624000478/xslForm13F_X02/primary_doc.xml" xr:uid="{CD16B160-C0FF-4B09-BDE9-92934FBD7269}"/>
     <hyperlink ref="R41" r:id="rId417" display="https://www.sec.gov/Archives/edgar/data/1503174/000090266424005141/xslForm13F_X02/primary_doc.xml" xr:uid="{37D7147E-0499-4379-BFEE-F04BF47E2CBC}"/>
     <hyperlink ref="B41" r:id="rId418" xr:uid="{D9E14C26-1E3B-4910-967E-8340D18B306B}"/>
     <hyperlink ref="B44" r:id="rId419" xr:uid="{0E455124-1E3A-47DD-A2E0-7CD3A86868DB}"/>
     <hyperlink ref="R44" r:id="rId420" display="https://www.sec.gov/Archives/edgar/data/1651424/000165142424000003/xslForm13F_X02/primary_doc.xml" xr:uid="{449A35F9-BBE6-4185-8C7D-687F84208A6C}"/>
-    <hyperlink ref="B72" r:id="rId421" xr:uid="{16CD0F2F-7A36-4556-9BAC-2FC6232B7FA0}"/>
-    <hyperlink ref="R72" r:id="rId422" display="https://www.sec.gov/Archives/edgar/data/1569064/000117266124003525/xslForm13F_X02/primary_doc.xml" xr:uid="{98FC0754-A402-444C-9CA2-9592C57DFEAC}"/>
+    <hyperlink ref="B73" r:id="rId421" xr:uid="{16CD0F2F-7A36-4556-9BAC-2FC6232B7FA0}"/>
+    <hyperlink ref="R73" r:id="rId422" display="https://www.sec.gov/Archives/edgar/data/1569064/000117266124003525/xslForm13F_X02/primary_doc.xml" xr:uid="{98FC0754-A402-444C-9CA2-9592C57DFEAC}"/>
+    <hyperlink ref="R90" r:id="rId423" display="https://www.sec.gov/Archives/edgar/data/1649339/000090514824002196/xslForm13F_X02/primary_doc.xml" xr:uid="{026DBB46-04C7-4B02-A2FC-03BAA70B5521}"/>
+    <hyperlink ref="B90" r:id="rId424" xr:uid="{C9082FBF-1E47-4917-9080-6DD7EE4630B5}"/>
+    <hyperlink ref="B49" r:id="rId425" xr:uid="{2D14AF52-817D-4CE4-9477-50B0F436572B}"/>
+    <hyperlink ref="R49" r:id="rId426" display="https://www.sec.gov/Archives/edgar/data/1510281/000106299324015052/xslForm13F_X02/primary_doc.xml" xr:uid="{4FF2BEB7-E396-4857-9C48-51CFB605FCC7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId423"/>
-  <legacyDrawing r:id="rId424"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId427"/>
+  <legacyDrawing r:id="rId428"/>
 </worksheet>
 </file>
 

</xml_diff>